<commit_message>
Added Eye and Hair code elements.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Custody_Query_Results/artifacts/service_model/information_model/IEPD/documentation/impl/CustodyQueryResults.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Custody_Query_Results/artifacts/service_model/information_model/IEPD/documentation/impl/CustodyQueryResults.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2010" yWindow="135" windowWidth="30045" windowHeight="16440" tabRatio="500"/>
+    <workbookView xWindow="-2520" yWindow="210" windowWidth="30045" windowHeight="16440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Custody Query Results Mappin" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="208">
   <si>
     <t>Race</t>
   </si>
@@ -402,12 +402,6 @@
     <t>Age</t>
   </si>
   <si>
-    <t>Eye Color</t>
-  </si>
-  <si>
-    <t>Hair Color</t>
-  </si>
-  <si>
     <t>Height</t>
   </si>
   <si>
@@ -631,6 +625,24 @@
   </si>
   <si>
     <t>/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/j:Booking[@structures:id=/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/j:ActivityCaseAssociation/nc:Activity/@structures:ref]/j:BookingAgencyRecordIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>Eye Color Text</t>
+  </si>
+  <si>
+    <t>Eye Color Code</t>
+  </si>
+  <si>
+    <t>Hair Color Code</t>
+  </si>
+  <si>
+    <t>Hair Color Text</t>
+  </si>
+  <si>
+    <t>/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/nc:Person[@structures:id=/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/j:PersonEyeColorCode</t>
+  </si>
+  <si>
+    <t>/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/nc:Person[@structures:id=/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/j:PersonHairColorCode</t>
   </si>
 </sst>
 </file>
@@ -2755,11 +2767,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R87"/>
+  <dimension ref="A1:R89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D52" sqref="D52"/>
+      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2774,7 +2786,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B1" s="30"/>
       <c r="C1" s="21"/>
@@ -2884,7 +2896,7 @@
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="14" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -2904,295 +2916,279 @@
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="5" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A13" s="15"/>
       <c r="B13" s="3" t="s">
-        <v>127</v>
+        <v>202</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="14" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="5" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
       <c r="B14" s="3" t="s">
-        <v>128</v>
+        <v>203</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="14" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" s="5" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="5" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
       <c r="B15" s="3" t="s">
-        <v>129</v>
+        <v>205</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="14" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" s="5" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="5" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A16" s="15"/>
       <c r="B16" s="3" t="s">
-        <v>130</v>
+        <v>204</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="14" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" s="5" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="5" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
       <c r="B17" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="14" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="63" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="14" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="5" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="A18" s="15"/>
+      <c r="B18" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="14" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="5" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="A19" s="15"/>
+      <c r="B19" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="14" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+      <c r="A20" s="14"/>
+      <c r="B20" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C20" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="14" t="s">
+      <c r="D20" s="8"/>
+      <c r="E20" s="14" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8" t="s">
+    <row r="21" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="B21" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C21" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14" t="s">
+      <c r="D21" s="14"/>
+      <c r="E21" s="14" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8" t="s">
+    <row r="22" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+      <c r="B22" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C22" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14" t="s">
+      <c r="D22" s="14"/>
+      <c r="E22" s="14" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="63" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="14" t="s">
+    <row r="23" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+      <c r="A23" s="14"/>
+      <c r="B23" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C23" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="14" t="s">
+      <c r="D23" s="8"/>
+      <c r="E23" s="14" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="63" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-      <c r="B22" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="63" x14ac:dyDescent="0.25">
-      <c r="A23" s="10"/>
-      <c r="B23" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="63" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="63" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
       <c r="B24" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>114</v>
+        <v>63</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>64</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="63" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="63" x14ac:dyDescent="0.25">
       <c r="A25" s="10"/>
       <c r="B25" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="63" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>66</v>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+      <c r="A26" s="10"/>
+      <c r="B26" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>114</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="63" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+      <c r="A27" s="10"/>
       <c r="B27" s="4" t="s">
-        <v>67</v>
+        <v>113</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>68</v>
+        <v>113</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="63" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="63" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
       <c r="B29" s="4" t="s">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" ht="63" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" s="13" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="D32" s="26"/>
-      <c r="E32" s="28" t="s">
-        <v>196</v>
-      </c>
-      <c r="F32" s="28"/>
-      <c r="G32" s="28"/>
-      <c r="H32" s="28"/>
-      <c r="I32" s="4"/>
-      <c r="J32" s="6"/>
-      <c r="K32" s="6"/>
-      <c r="L32" s="6"/>
-      <c r="M32" s="6"/>
-    </row>
-    <row r="33" spans="1:13" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="63" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4" t="s">
-        <v>194</v>
+        <v>104</v>
       </c>
       <c r="C33" s="4"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="F33" s="27"/>
-      <c r="G33" s="28"/>
-      <c r="H33" s="28"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="6"/>
-      <c r="K33" s="6"/>
-      <c r="L33" s="6"/>
-      <c r="M33" s="6"/>
-    </row>
-    <row r="34" spans="1:13" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="D33" s="10"/>
+      <c r="E33" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" s="13" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="C34" s="4"/>
+        <v>190</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>191</v>
+      </c>
       <c r="D34" s="26"/>
-      <c r="E34" s="8" t="s">
-        <v>200</v>
-      </c>
-      <c r="F34" s="27"/>
+      <c r="E34" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="F34" s="28"/>
       <c r="G34" s="28"/>
       <c r="H34" s="28"/>
       <c r="I34" s="4"/>
@@ -3204,12 +3200,12 @@
     <row r="35" spans="1:13" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C35" s="4"/>
       <c r="D35" s="26"/>
-      <c r="E35" s="8" t="s">
-        <v>198</v>
+      <c r="E35" s="6" t="s">
+        <v>195</v>
       </c>
       <c r="F35" s="27"/>
       <c r="G35" s="28"/>
@@ -3220,448 +3216,438 @@
       <c r="L35" s="6"/>
       <c r="M35" s="6"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="12" t="s">
+    <row r="36" spans="1:13" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="C36" s="4"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="F36" s="27"/>
+      <c r="G36" s="28"/>
+      <c r="H36" s="28"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="6"/>
+      <c r="K36" s="6"/>
+      <c r="L36" s="6"/>
+      <c r="M36" s="6"/>
+    </row>
+    <row r="37" spans="1:13" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="C37" s="4"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="F37" s="27"/>
+      <c r="G37" s="28"/>
+      <c r="H37" s="28"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="6"/>
+      <c r="K37" s="6"/>
+      <c r="L37" s="6"/>
+      <c r="M37" s="6"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-    </row>
-    <row r="37" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B37" s="4" t="s">
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B39" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C39" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E37" s="9" t="s">
+      <c r="E39" s="9" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B38" s="3" t="s">
+    <row r="40" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B40" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C40" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E38" s="9" t="s">
+      <c r="E40" s="9" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="5"/>
-      <c r="B39" s="5" t="s">
+    <row r="41" spans="1:13" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="5"/>
+      <c r="B41" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C41" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D39" s="5"/>
-      <c r="E39" s="7" t="s">
+      <c r="D41" s="5"/>
+      <c r="E41" s="7" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="12" t="s">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-    </row>
-    <row r="41" spans="1:13" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
-      <c r="A41" s="29"/>
-      <c r="B41" s="4" t="s">
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+    </row>
+    <row r="43" spans="1:13" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="A43" s="29"/>
+      <c r="B43" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="14" t="s">
         <v>201</v>
       </c>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="14" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" ht="63" x14ac:dyDescent="0.25">
-      <c r="A42" s="16"/>
-      <c r="B42" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="C42" s="14" t="s">
+    </row>
+    <row r="44" spans="1:13" ht="63" x14ac:dyDescent="0.25">
+      <c r="A44" s="16"/>
+      <c r="B44" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="C44" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14" t="s">
+      <c r="D44" s="14"/>
+      <c r="E44" s="14" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A45" s="14"/>
+      <c r="B45" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D45" s="8"/>
+      <c r="E45" s="14" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="63" x14ac:dyDescent="0.25">
+      <c r="A46" s="14"/>
+      <c r="B46" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="C46" s="8" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A43" s="14"/>
-      <c r="B43" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="D43" s="8"/>
-      <c r="E43" s="14" t="s">
+      <c r="D46" s="8"/>
+      <c r="E46" s="14" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="63" x14ac:dyDescent="0.25">
+      <c r="B47" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E47" s="14" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+    </row>
+    <row r="49" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A49" s="5"/>
+      <c r="B49" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A50" s="5"/>
+      <c r="B50" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D50" s="5"/>
+      <c r="E50" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+    </row>
+    <row r="52" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+      <c r="B52" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B53" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E53" s="9" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E54" s="2" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="63" x14ac:dyDescent="0.25">
-      <c r="A44" s="14"/>
-      <c r="B44" s="8" t="s">
-        <v>186</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="D44" s="8"/>
-      <c r="E44" s="14" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" ht="63" x14ac:dyDescent="0.25">
-      <c r="B45" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E45" s="14" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A46" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-    </row>
-    <row r="47" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A47" s="5"/>
-      <c r="B47" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A48" s="5"/>
-      <c r="B48" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D48" s="5"/>
-      <c r="E48" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-    </row>
-    <row r="50" spans="1:5" ht="63" x14ac:dyDescent="0.25">
-      <c r="B50" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E50" s="2" t="s">
+    <row r="55" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+      <c r="B55" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="A56" s="8"/>
+      <c r="B56" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C56" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="E56" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B51" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E51" s="9" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="63" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="63" x14ac:dyDescent="0.25">
-      <c r="B53" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E53" s="2" t="s">
+    <row r="57" spans="1:5" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="A57" s="8"/>
+      <c r="B57" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="C57" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="E57" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="54" spans="1:5" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
-      <c r="A54" s="8"/>
-      <c r="B54" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="C54" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
-      <c r="A55" s="8"/>
-      <c r="B55" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="C55" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="63" x14ac:dyDescent="0.25">
-      <c r="A56" s="5"/>
-      <c r="B56" s="6" t="s">
+    <row r="58" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+      <c r="A58" s="5"/>
+      <c r="B58" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C56" s="5" t="s">
+      <c r="C58" s="5" t="s">
         <v>48</v>
-      </c>
-      <c r="D56" s="5"/>
-      <c r="E56" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="63" x14ac:dyDescent="0.25">
-      <c r="A57" s="5"/>
-      <c r="B57" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
-      <c r="E57" s="5" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="63" x14ac:dyDescent="0.25">
-      <c r="A58" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>50</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="5" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A59" s="5" t="s">
-        <v>38</v>
-      </c>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+      <c r="A59" s="5"/>
       <c r="B59" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>52</v>
-      </c>
+        <v>187</v>
+      </c>
+      <c r="C59" s="5"/>
       <c r="D59" s="5"/>
       <c r="E59" s="5" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="12" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+      <c r="A60" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D60" s="5"/>
+      <c r="E60" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A61" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D61" s="5"/>
+      <c r="E61" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B60" s="24"/>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
-      <c r="E60" s="1"/>
-    </row>
-    <row r="61" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B61" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E61" s="14" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B62" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="E62" s="14" t="s">
-        <v>162</v>
-      </c>
+      <c r="B62" s="24"/>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
     </row>
     <row r="63" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B63" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E63" s="14" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B64" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E64" s="14" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B65" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="C65" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E63" s="14" t="s">
+      <c r="E65" s="14" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18" ht="63" x14ac:dyDescent="0.25">
+      <c r="B66" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E66" s="14" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" ht="63" x14ac:dyDescent="0.25">
+      <c r="B67" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E67" s="14" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="63" x14ac:dyDescent="0.25">
-      <c r="B64" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E64" s="14" t="s">
+    <row r="68" spans="1:18" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A68" s="5"/>
+      <c r="B68" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D68" s="6"/>
+      <c r="E68" s="5" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="65" spans="1:18" ht="63" x14ac:dyDescent="0.25">
-      <c r="B65" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="E65" s="14" t="s">
+    <row r="69" spans="1:18" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="5"/>
+      <c r="B69" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
+      <c r="E69" s="14" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="66" spans="1:18" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A66" s="5"/>
-      <c r="B66" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C66" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D66" s="6"/>
-      <c r="E66" s="5" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="67" spans="1:18" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="5"/>
-      <c r="B67" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="C67" s="5"/>
-      <c r="D67" s="5"/>
-      <c r="E67" s="14" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="68" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A68" s="5" t="s">
+    <row r="70" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A70" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B70" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C68" s="5" t="s">
+      <c r="C70" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D68" s="5"/>
-      <c r="E68" s="5" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A69" s="12" t="s">
+      <c r="D70" s="5"/>
+      <c r="E70" s="5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A71" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B69" s="24"/>
-      <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
-    </row>
-    <row r="70" spans="1:18" s="13" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A70" s="6"/>
-      <c r="B70" s="25" t="s">
-        <v>172</v>
-      </c>
-      <c r="C70" s="6"/>
-      <c r="D70" s="22"/>
-      <c r="E70" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="F70" s="23"/>
-      <c r="G70" s="23"/>
-      <c r="H70" s="23"/>
-      <c r="I70" s="4"/>
-      <c r="J70" s="6"/>
-      <c r="K70" s="6"/>
-      <c r="L70" s="6"/>
-      <c r="M70" s="6"/>
-      <c r="N70" s="6"/>
-      <c r="O70" s="6"/>
-      <c r="P70" s="6"/>
-      <c r="Q70" s="6"/>
-      <c r="R70" s="6"/>
-    </row>
-    <row r="71" spans="1:18" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
-      <c r="A71" s="6"/>
-      <c r="B71" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="C71" s="6"/>
-      <c r="D71" s="22"/>
-      <c r="E71" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="F71" s="23"/>
-      <c r="G71" s="23"/>
-      <c r="H71" s="23"/>
-      <c r="I71" s="4"/>
-      <c r="J71" s="6"/>
-      <c r="K71" s="6"/>
-      <c r="L71" s="6"/>
-      <c r="M71" s="6"/>
-      <c r="N71" s="6"/>
-      <c r="O71" s="6"/>
-      <c r="P71" s="6"/>
-      <c r="Q71" s="6"/>
-      <c r="R71" s="6"/>
+      <c r="B71" s="24"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
     </row>
     <row r="72" spans="1:18" s="13" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A72" s="6"/>
       <c r="B72" s="25" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C72" s="6"/>
       <c r="D72" s="22"/>
@@ -3682,10 +3668,10 @@
       <c r="Q72" s="6"/>
       <c r="R72" s="6"/>
     </row>
-    <row r="73" spans="1:18" s="13" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:18" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A73" s="6"/>
       <c r="B73" s="25" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C73" s="6"/>
       <c r="D73" s="22"/>
@@ -3706,10 +3692,10 @@
       <c r="Q73" s="6"/>
       <c r="R73" s="6"/>
     </row>
-    <row r="74" spans="1:18" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:18" s="13" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A74" s="6"/>
       <c r="B74" s="25" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C74" s="6"/>
       <c r="D74" s="22"/>
@@ -3733,7 +3719,7 @@
     <row r="75" spans="1:18" s="13" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A75" s="6"/>
       <c r="B75" s="25" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C75" s="6"/>
       <c r="D75" s="22"/>
@@ -3754,119 +3740,167 @@
       <c r="Q75" s="6"/>
       <c r="R75" s="6"/>
     </row>
-    <row r="76" spans="1:18" ht="63" x14ac:dyDescent="0.25">
-      <c r="A76" s="5"/>
-      <c r="B76" s="6" t="s">
-        <v>105</v>
+    <row r="76" spans="1:18" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="A76" s="6"/>
+      <c r="B76" s="25" t="s">
+        <v>174</v>
       </c>
       <c r="C76" s="6"/>
-      <c r="D76" s="11"/>
+      <c r="D76" s="22"/>
       <c r="E76" s="3" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="77" spans="1:18" ht="63" x14ac:dyDescent="0.25">
-      <c r="A77" s="5"/>
-      <c r="B77" s="6" t="s">
-        <v>106</v>
+      <c r="F76" s="23"/>
+      <c r="G76" s="23"/>
+      <c r="H76" s="23"/>
+      <c r="I76" s="4"/>
+      <c r="J76" s="6"/>
+      <c r="K76" s="6"/>
+      <c r="L76" s="6"/>
+      <c r="M76" s="6"/>
+      <c r="N76" s="6"/>
+      <c r="O76" s="6"/>
+      <c r="P76" s="6"/>
+      <c r="Q76" s="6"/>
+      <c r="R76" s="6"/>
+    </row>
+    <row r="77" spans="1:18" s="13" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A77" s="6"/>
+      <c r="B77" s="25" t="s">
+        <v>175</v>
       </c>
       <c r="C77" s="6"/>
-      <c r="D77" s="11"/>
+      <c r="D77" s="22"/>
       <c r="E77" s="3" t="s">
-        <v>108</v>
-      </c>
+        <v>177</v>
+      </c>
+      <c r="F77" s="23"/>
+      <c r="G77" s="23"/>
+      <c r="H77" s="23"/>
+      <c r="I77" s="4"/>
+      <c r="J77" s="6"/>
+      <c r="K77" s="6"/>
+      <c r="L77" s="6"/>
+      <c r="M77" s="6"/>
+      <c r="N77" s="6"/>
+      <c r="O77" s="6"/>
+      <c r="P77" s="6"/>
+      <c r="Q77" s="6"/>
+      <c r="R77" s="6"/>
     </row>
     <row r="78" spans="1:18" ht="63" x14ac:dyDescent="0.25">
       <c r="A78" s="5"/>
       <c r="B78" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C78" s="6"/>
+      <c r="D78" s="11"/>
+      <c r="E78" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18" ht="63" x14ac:dyDescent="0.25">
+      <c r="A79" s="5"/>
+      <c r="B79" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C79" s="6"/>
+      <c r="D79" s="11"/>
+      <c r="E79" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" ht="63" x14ac:dyDescent="0.25">
+      <c r="A80" s="5"/>
+      <c r="B80" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C78" s="5" t="s">
+      <c r="C80" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D78" s="5"/>
-      <c r="E78" s="5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A79" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="B79" s="24"/>
-      <c r="C79" s="1"/>
-      <c r="D79" s="1"/>
-      <c r="E79" s="1"/>
-    </row>
-    <row r="80" spans="1:18" s="13" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B80" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="E80" s="13" t="s">
-        <v>169</v>
+      <c r="D80" s="5"/>
+      <c r="E80" s="5" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="12" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="B81" s="24"/>
       <c r="C81" s="1"/>
-      <c r="D81" s="17"/>
+      <c r="D81" s="1"/>
       <c r="E81" s="1"/>
     </row>
-    <row r="82" spans="1:5" ht="63" x14ac:dyDescent="0.25">
-      <c r="B82" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="D82" s="18"/>
-      <c r="E82" s="8" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" ht="63" x14ac:dyDescent="0.25">
-      <c r="B83" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="D83" s="18"/>
-      <c r="E83" s="8" t="s">
-        <v>170</v>
-      </c>
+    <row r="82" spans="1:5" s="13" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B82" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="E82" s="13" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="B83" s="24"/>
+      <c r="C83" s="1"/>
+      <c r="D83" s="17"/>
+      <c r="E83" s="1"/>
     </row>
     <row r="84" spans="1:5" ht="63" x14ac:dyDescent="0.25">
       <c r="B84" s="13" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D84" s="18"/>
       <c r="E84" s="8" t="s">
-        <v>171</v>
+        <v>146</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="63" x14ac:dyDescent="0.25">
       <c r="B85" s="13" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D85" s="18"/>
       <c r="E85" s="8" t="s">
-        <v>145</v>
+        <v>168</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="63" x14ac:dyDescent="0.25">
       <c r="B86" s="13" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D86" s="18"/>
       <c r="E86" s="8" t="s">
-        <v>146</v>
+        <v>169</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="63" x14ac:dyDescent="0.25">
       <c r="B87" s="13" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D87" s="18"/>
       <c r="E87" s="8" t="s">
-        <v>147</v>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+      <c r="B88" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="D88" s="18"/>
+      <c r="E88" s="8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+      <c r="B89" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="D89" s="18"/>
+      <c r="E89" s="8" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Aliases (nc:Identity) to the IEPD.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Custody_Query_Results/artifacts/service_model/information_model/IEPD/documentation/impl/CustodyQueryResults.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Custody_Query_Results/artifacts/service_model/information_model/IEPD/documentation/impl/CustodyQueryResults.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-2520" yWindow="210" windowWidth="30045" windowHeight="16440" tabRatio="500"/>
+    <workbookView xWindow="2070" yWindow="465" windowWidth="20580" windowHeight="9870" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Custody Query Results Mappin" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="214">
   <si>
     <t>Race</t>
   </si>
@@ -643,13 +643,31 @@
   </si>
   <si>
     <t>/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/nc:Person[@structures:id=/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/j:PersonHairColorCode</t>
+  </si>
+  <si>
+    <t>Alias</t>
+  </si>
+  <si>
+    <t>/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/nc:Identity[@structures:id=/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/nc:PersonAliasIdentityAssociation/nc:Identity/@structures:ref]/nc:IdentityPersonRepresentation/nc:PersonBirthDate/nc:Date</t>
+  </si>
+  <si>
+    <t>/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/nc:Identity[@structures:id=/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/nc:PersonAliasIdentityAssociation/nc:Identity/@structures:ref]/nc:IdentityPersonRepresentation/nc:PersonName/nc:PersonGivenName</t>
+  </si>
+  <si>
+    <t>/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/nc:Identity[@structures:id=/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/nc:PersonAliasIdentityAssociation/nc:Identity/@structures:ref]/nc:IdentityPersonRepresentation/nc:PersonName/nc:PersonMiddleName</t>
+  </si>
+  <si>
+    <t>/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/nc:Identity[@structures:id=/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/nc:PersonAliasIdentityAssociation/nc:Identity/@structures:ref]/nc:IdentityPersonRepresentation/nc:PersonName/nc:PersonSurName</t>
+  </si>
+  <si>
+    <t>/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/nc:Identity[@structures:id=/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/nc:PersonAliasIdentityAssociation/nc:Identity/@structures:ref]/nc:IdentityPersonRepresentation/j:PersonSexCode</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -735,6 +753,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1556,7 +1580,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1644,6 +1668,12 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="707" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2767,11 +2797,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R89"/>
+  <dimension ref="A1:R95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+      <pane ySplit="2" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2785,10 +2815,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="B1" s="30"/>
+      <c r="B1" s="32"/>
       <c r="C1" s="21"/>
       <c r="D1" s="21"/>
       <c r="E1" s="21"/>
@@ -3254,652 +3284,726 @@
       <c r="L37" s="6"/>
       <c r="M37" s="6"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" s="12" t="s">
+    <row r="38" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="30" t="s">
+        <v>208</v>
+      </c>
+      <c r="B38" s="24"/>
+      <c r="C38" s="24"/>
+      <c r="D38" s="24"/>
+      <c r="E38" s="24"/>
+    </row>
+    <row r="39" spans="1:13" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="A39" s="8"/>
+      <c r="B39" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D39" s="8"/>
+      <c r="E39" s="31" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="A40" s="8"/>
+      <c r="B40" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D40" s="8"/>
+      <c r="E40" s="31" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="A41" s="8"/>
+      <c r="B41" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D41" s="8"/>
+      <c r="E41" s="31" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="A42" s="8"/>
+      <c r="B42" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D42" s="8"/>
+      <c r="E42" s="31" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="A43" s="8"/>
+      <c r="B43" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D43" s="8"/>
+      <c r="E43" s="31" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-    </row>
-    <row r="39" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B39" s="4" t="s">
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+    </row>
+    <row r="45" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B45" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C45" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E39" s="9" t="s">
+      <c r="E45" s="9" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B40" s="3" t="s">
+    <row r="46" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B46" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C46" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E40" s="9" t="s">
+      <c r="E46" s="9" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5" t="s">
+    <row r="47" spans="1:13" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="5"/>
+      <c r="B47" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C47" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D41" s="5"/>
-      <c r="E41" s="7" t="s">
+      <c r="D47" s="5"/>
+      <c r="E47" s="7" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-    </row>
-    <row r="43" spans="1:13" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
-      <c r="A43" s="29"/>
-      <c r="B43" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="14" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" ht="63" x14ac:dyDescent="0.25">
-      <c r="A44" s="16"/>
-      <c r="B44" s="8" t="s">
-        <v>200</v>
-      </c>
-      <c r="C44" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="D44" s="14"/>
-      <c r="E44" s="14" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A45" s="14"/>
-      <c r="B45" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="D45" s="8"/>
-      <c r="E45" s="14" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" ht="63" x14ac:dyDescent="0.25">
-      <c r="A46" s="14"/>
-      <c r="B46" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="D46" s="8"/>
-      <c r="E46" s="14" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" ht="63" x14ac:dyDescent="0.25">
-      <c r="B47" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E47" s="14" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
     </row>
-    <row r="49" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A49" s="5"/>
-      <c r="B49" s="5" t="s">
+    <row r="49" spans="1:5" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="A49" s="29"/>
+      <c r="B49" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="14" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+      <c r="A50" s="16"/>
+      <c r="B50" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="C50" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A51" s="14"/>
+      <c r="B51" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D51" s="8"/>
+      <c r="E51" s="14" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+      <c r="A52" s="14"/>
+      <c r="B52" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="D52" s="8"/>
+      <c r="E52" s="14" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+      <c r="B53" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E53" s="14" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+    </row>
+    <row r="55" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A55" s="5"/>
+      <c r="B55" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="3" t="s">
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="3" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A50" s="5"/>
-      <c r="B50" s="4" t="s">
+    <row r="56" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A56" s="5"/>
+      <c r="B56" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C50" s="5" t="s">
+      <c r="C56" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D50" s="5"/>
-      <c r="E50" s="3" t="s">
+      <c r="D56" s="5"/>
+      <c r="E56" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="12" t="s">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-    </row>
-    <row r="52" spans="1:5" ht="63" x14ac:dyDescent="0.25">
-      <c r="B52" s="4" t="s">
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+    </row>
+    <row r="58" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+      <c r="B58" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C58" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E52" s="2" t="s">
+      <c r="E58" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B53" s="4" t="s">
+    <row r="59" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B59" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C59" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E53" s="9" t="s">
+      <c r="E59" s="9" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="63" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
+    <row r="60" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B60" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="C60" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E54" s="2" t="s">
+      <c r="E60" s="2" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="63" x14ac:dyDescent="0.25">
-      <c r="B55" s="4" t="s">
+    <row r="61" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+      <c r="B61" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="C61" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E55" s="2" t="s">
+      <c r="E61" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="56" spans="1:5" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
-      <c r="A56" s="8"/>
-      <c r="B56" s="8" t="s">
+    <row r="62" spans="1:5" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="A62" s="8"/>
+      <c r="B62" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="C56" s="13" t="s">
+      <c r="C62" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="E56" s="2" t="s">
+      <c r="E62" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="57" spans="1:5" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
-      <c r="A57" s="8"/>
-      <c r="B57" s="13" t="s">
+    <row r="63" spans="1:5" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="A63" s="8"/>
+      <c r="B63" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="C57" s="13" t="s">
+      <c r="C63" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="E57" s="2" t="s">
+      <c r="E63" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="63" x14ac:dyDescent="0.25">
-      <c r="A58" s="5"/>
-      <c r="B58" s="6" t="s">
+    <row r="64" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+      <c r="A64" s="5"/>
+      <c r="B64" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C58" s="5" t="s">
+      <c r="C64" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D58" s="5"/>
-      <c r="E58" s="5" t="s">
+      <c r="D64" s="5"/>
+      <c r="E64" s="5" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="63" x14ac:dyDescent="0.25">
-      <c r="A59" s="5"/>
-      <c r="B59" s="6" t="s">
+    <row r="65" spans="1:18" ht="63" x14ac:dyDescent="0.25">
+      <c r="A65" s="5"/>
+      <c r="B65" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="C59" s="5"/>
-      <c r="D59" s="5"/>
-      <c r="E59" s="5" t="s">
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
+      <c r="E65" s="5" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="63" x14ac:dyDescent="0.25">
-      <c r="A60" s="5" t="s">
+    <row r="66" spans="1:18" ht="63" x14ac:dyDescent="0.25">
+      <c r="A66" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B60" s="6" t="s">
+      <c r="B66" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C60" s="5" t="s">
+      <c r="C66" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D60" s="5"/>
-      <c r="E60" s="5" t="s">
+      <c r="D66" s="5"/>
+      <c r="E66" s="5" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A61" s="5" t="s">
+    <row r="67" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A67" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B61" s="6" t="s">
+      <c r="B67" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C61" s="5" t="s">
+      <c r="C67" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D61" s="5"/>
-      <c r="E61" s="5" t="s">
+      <c r="D67" s="5"/>
+      <c r="E67" s="5" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="12" t="s">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A68" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B62" s="24"/>
-      <c r="C62" s="1"/>
-      <c r="D62" s="1"/>
-      <c r="E62" s="1"/>
-    </row>
-    <row r="63" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B63" s="4" t="s">
+      <c r="B68" s="24"/>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+    </row>
+    <row r="69" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B69" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="C69" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E63" s="14" t="s">
+      <c r="E69" s="14" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B64" s="4" t="s">
+    <row r="70" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B70" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="E64" s="14" t="s">
+      <c r="E70" s="14" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="65" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B65" s="4" t="s">
+    <row r="71" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B71" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="C71" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E65" s="14" t="s">
+      <c r="E71" s="14" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="66" spans="1:18" ht="63" x14ac:dyDescent="0.25">
-      <c r="B66" s="4" t="s">
+    <row r="72" spans="1:18" ht="63" x14ac:dyDescent="0.25">
+      <c r="B72" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C72" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E66" s="14" t="s">
+      <c r="E72" s="14" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="67" spans="1:18" ht="63" x14ac:dyDescent="0.25">
-      <c r="B67" s="4" t="s">
+    <row r="73" spans="1:18" ht="63" x14ac:dyDescent="0.25">
+      <c r="B73" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="C73" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="E67" s="14" t="s">
+      <c r="E73" s="14" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="68" spans="1:18" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A68" s="5"/>
-      <c r="B68" s="6" t="s">
+    <row r="74" spans="1:18" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A74" s="5"/>
+      <c r="B74" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C68" s="6" t="s">
+      <c r="C74" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D68" s="6"/>
-      <c r="E68" s="5" t="s">
+      <c r="D74" s="6"/>
+      <c r="E74" s="5" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="69" spans="1:18" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="5"/>
-      <c r="B69" s="6" t="s">
+    <row r="75" spans="1:18" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="5"/>
+      <c r="B75" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C69" s="5"/>
-      <c r="D69" s="5"/>
-      <c r="E69" s="14" t="s">
+      <c r="C75" s="5"/>
+      <c r="D75" s="5"/>
+      <c r="E75" s="14" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="70" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A70" s="5" t="s">
+    <row r="76" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A76" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B76" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C70" s="5" t="s">
+      <c r="C76" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D70" s="5"/>
-      <c r="E70" s="5" t="s">
+      <c r="D76" s="5"/>
+      <c r="E76" s="5" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A71" s="12" t="s">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A77" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B71" s="24"/>
-      <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
-      <c r="E71" s="1"/>
-    </row>
-    <row r="72" spans="1:18" s="13" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A72" s="6"/>
-      <c r="B72" s="25" t="s">
+      <c r="B77" s="24"/>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
+    </row>
+    <row r="78" spans="1:18" s="13" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A78" s="6"/>
+      <c r="B78" s="25" t="s">
         <v>170</v>
       </c>
-      <c r="C72" s="6"/>
-      <c r="D72" s="22"/>
-      <c r="E72" s="3" t="s">
+      <c r="C78" s="6"/>
+      <c r="D78" s="22"/>
+      <c r="E78" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="F72" s="23"/>
-      <c r="G72" s="23"/>
-      <c r="H72" s="23"/>
-      <c r="I72" s="4"/>
-      <c r="J72" s="6"/>
-      <c r="K72" s="6"/>
-      <c r="L72" s="6"/>
-      <c r="M72" s="6"/>
-      <c r="N72" s="6"/>
-      <c r="O72" s="6"/>
-      <c r="P72" s="6"/>
-      <c r="Q72" s="6"/>
-      <c r="R72" s="6"/>
-    </row>
-    <row r="73" spans="1:18" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
-      <c r="A73" s="6"/>
-      <c r="B73" s="25" t="s">
+      <c r="F78" s="23"/>
+      <c r="G78" s="23"/>
+      <c r="H78" s="23"/>
+      <c r="I78" s="4"/>
+      <c r="J78" s="6"/>
+      <c r="K78" s="6"/>
+      <c r="L78" s="6"/>
+      <c r="M78" s="6"/>
+      <c r="N78" s="6"/>
+      <c r="O78" s="6"/>
+      <c r="P78" s="6"/>
+      <c r="Q78" s="6"/>
+      <c r="R78" s="6"/>
+    </row>
+    <row r="79" spans="1:18" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="A79" s="6"/>
+      <c r="B79" s="25" t="s">
         <v>171</v>
       </c>
-      <c r="C73" s="6"/>
-      <c r="D73" s="22"/>
-      <c r="E73" s="3" t="s">
+      <c r="C79" s="6"/>
+      <c r="D79" s="22"/>
+      <c r="E79" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="F73" s="23"/>
-      <c r="G73" s="23"/>
-      <c r="H73" s="23"/>
-      <c r="I73" s="4"/>
-      <c r="J73" s="6"/>
-      <c r="K73" s="6"/>
-      <c r="L73" s="6"/>
-      <c r="M73" s="6"/>
-      <c r="N73" s="6"/>
-      <c r="O73" s="6"/>
-      <c r="P73" s="6"/>
-      <c r="Q73" s="6"/>
-      <c r="R73" s="6"/>
-    </row>
-    <row r="74" spans="1:18" s="13" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A74" s="6"/>
-      <c r="B74" s="25" t="s">
+      <c r="F79" s="23"/>
+      <c r="G79" s="23"/>
+      <c r="H79" s="23"/>
+      <c r="I79" s="4"/>
+      <c r="J79" s="6"/>
+      <c r="K79" s="6"/>
+      <c r="L79" s="6"/>
+      <c r="M79" s="6"/>
+      <c r="N79" s="6"/>
+      <c r="O79" s="6"/>
+      <c r="P79" s="6"/>
+      <c r="Q79" s="6"/>
+      <c r="R79" s="6"/>
+    </row>
+    <row r="80" spans="1:18" s="13" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A80" s="6"/>
+      <c r="B80" s="25" t="s">
         <v>172</v>
       </c>
-      <c r="C74" s="6"/>
-      <c r="D74" s="22"/>
-      <c r="E74" s="3" t="s">
+      <c r="C80" s="6"/>
+      <c r="D80" s="22"/>
+      <c r="E80" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="F74" s="23"/>
-      <c r="G74" s="23"/>
-      <c r="H74" s="23"/>
-      <c r="I74" s="4"/>
-      <c r="J74" s="6"/>
-      <c r="K74" s="6"/>
-      <c r="L74" s="6"/>
-      <c r="M74" s="6"/>
-      <c r="N74" s="6"/>
-      <c r="O74" s="6"/>
-      <c r="P74" s="6"/>
-      <c r="Q74" s="6"/>
-      <c r="R74" s="6"/>
-    </row>
-    <row r="75" spans="1:18" s="13" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A75" s="6"/>
-      <c r="B75" s="25" t="s">
+      <c r="F80" s="23"/>
+      <c r="G80" s="23"/>
+      <c r="H80" s="23"/>
+      <c r="I80" s="4"/>
+      <c r="J80" s="6"/>
+      <c r="K80" s="6"/>
+      <c r="L80" s="6"/>
+      <c r="M80" s="6"/>
+      <c r="N80" s="6"/>
+      <c r="O80" s="6"/>
+      <c r="P80" s="6"/>
+      <c r="Q80" s="6"/>
+      <c r="R80" s="6"/>
+    </row>
+    <row r="81" spans="1:18" s="13" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A81" s="6"/>
+      <c r="B81" s="25" t="s">
         <v>173</v>
       </c>
-      <c r="C75" s="6"/>
-      <c r="D75" s="22"/>
-      <c r="E75" s="3" t="s">
+      <c r="C81" s="6"/>
+      <c r="D81" s="22"/>
+      <c r="E81" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="F75" s="23"/>
-      <c r="G75" s="23"/>
-      <c r="H75" s="23"/>
-      <c r="I75" s="4"/>
-      <c r="J75" s="6"/>
-      <c r="K75" s="6"/>
-      <c r="L75" s="6"/>
-      <c r="M75" s="6"/>
-      <c r="N75" s="6"/>
-      <c r="O75" s="6"/>
-      <c r="P75" s="6"/>
-      <c r="Q75" s="6"/>
-      <c r="R75" s="6"/>
-    </row>
-    <row r="76" spans="1:18" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
-      <c r="A76" s="6"/>
-      <c r="B76" s="25" t="s">
+      <c r="F81" s="23"/>
+      <c r="G81" s="23"/>
+      <c r="H81" s="23"/>
+      <c r="I81" s="4"/>
+      <c r="J81" s="6"/>
+      <c r="K81" s="6"/>
+      <c r="L81" s="6"/>
+      <c r="M81" s="6"/>
+      <c r="N81" s="6"/>
+      <c r="O81" s="6"/>
+      <c r="P81" s="6"/>
+      <c r="Q81" s="6"/>
+      <c r="R81" s="6"/>
+    </row>
+    <row r="82" spans="1:18" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="A82" s="6"/>
+      <c r="B82" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="C76" s="6"/>
-      <c r="D76" s="22"/>
-      <c r="E76" s="3" t="s">
+      <c r="C82" s="6"/>
+      <c r="D82" s="22"/>
+      <c r="E82" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="F76" s="23"/>
-      <c r="G76" s="23"/>
-      <c r="H76" s="23"/>
-      <c r="I76" s="4"/>
-      <c r="J76" s="6"/>
-      <c r="K76" s="6"/>
-      <c r="L76" s="6"/>
-      <c r="M76" s="6"/>
-      <c r="N76" s="6"/>
-      <c r="O76" s="6"/>
-      <c r="P76" s="6"/>
-      <c r="Q76" s="6"/>
-      <c r="R76" s="6"/>
-    </row>
-    <row r="77" spans="1:18" s="13" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A77" s="6"/>
-      <c r="B77" s="25" t="s">
+      <c r="F82" s="23"/>
+      <c r="G82" s="23"/>
+      <c r="H82" s="23"/>
+      <c r="I82" s="4"/>
+      <c r="J82" s="6"/>
+      <c r="K82" s="6"/>
+      <c r="L82" s="6"/>
+      <c r="M82" s="6"/>
+      <c r="N82" s="6"/>
+      <c r="O82" s="6"/>
+      <c r="P82" s="6"/>
+      <c r="Q82" s="6"/>
+      <c r="R82" s="6"/>
+    </row>
+    <row r="83" spans="1:18" s="13" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A83" s="6"/>
+      <c r="B83" s="25" t="s">
         <v>175</v>
       </c>
-      <c r="C77" s="6"/>
-      <c r="D77" s="22"/>
-      <c r="E77" s="3" t="s">
+      <c r="C83" s="6"/>
+      <c r="D83" s="22"/>
+      <c r="E83" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="F77" s="23"/>
-      <c r="G77" s="23"/>
-      <c r="H77" s="23"/>
-      <c r="I77" s="4"/>
-      <c r="J77" s="6"/>
-      <c r="K77" s="6"/>
-      <c r="L77" s="6"/>
-      <c r="M77" s="6"/>
-      <c r="N77" s="6"/>
-      <c r="O77" s="6"/>
-      <c r="P77" s="6"/>
-      <c r="Q77" s="6"/>
-      <c r="R77" s="6"/>
-    </row>
-    <row r="78" spans="1:18" ht="63" x14ac:dyDescent="0.25">
-      <c r="A78" s="5"/>
-      <c r="B78" s="6" t="s">
+      <c r="F83" s="23"/>
+      <c r="G83" s="23"/>
+      <c r="H83" s="23"/>
+      <c r="I83" s="4"/>
+      <c r="J83" s="6"/>
+      <c r="K83" s="6"/>
+      <c r="L83" s="6"/>
+      <c r="M83" s="6"/>
+      <c r="N83" s="6"/>
+      <c r="O83" s="6"/>
+      <c r="P83" s="6"/>
+      <c r="Q83" s="6"/>
+      <c r="R83" s="6"/>
+    </row>
+    <row r="84" spans="1:18" ht="63" x14ac:dyDescent="0.25">
+      <c r="A84" s="5"/>
+      <c r="B84" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="C78" s="6"/>
-      <c r="D78" s="11"/>
-      <c r="E78" s="3" t="s">
+      <c r="C84" s="6"/>
+      <c r="D84" s="11"/>
+      <c r="E84" s="3" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="79" spans="1:18" ht="63" x14ac:dyDescent="0.25">
-      <c r="A79" s="5"/>
-      <c r="B79" s="6" t="s">
+    <row r="85" spans="1:18" ht="63" x14ac:dyDescent="0.25">
+      <c r="A85" s="5"/>
+      <c r="B85" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="C79" s="6"/>
-      <c r="D79" s="11"/>
-      <c r="E79" s="3" t="s">
+      <c r="C85" s="6"/>
+      <c r="D85" s="11"/>
+      <c r="E85" s="3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="80" spans="1:18" ht="63" x14ac:dyDescent="0.25">
-      <c r="A80" s="5"/>
-      <c r="B80" s="6" t="s">
+    <row r="86" spans="1:18" ht="63" x14ac:dyDescent="0.25">
+      <c r="A86" s="5"/>
+      <c r="B86" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C80" s="5" t="s">
+      <c r="C86" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D80" s="5"/>
-      <c r="E80" s="5" t="s">
+      <c r="D86" s="5"/>
+      <c r="E86" s="5" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="12" t="s">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A87" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="B81" s="24"/>
-      <c r="C81" s="1"/>
-      <c r="D81" s="1"/>
-      <c r="E81" s="1"/>
-    </row>
-    <row r="82" spans="1:5" s="13" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B82" s="4" t="s">
+      <c r="B87" s="24"/>
+      <c r="C87" s="1"/>
+      <c r="D87" s="1"/>
+      <c r="E87" s="1"/>
+    </row>
+    <row r="88" spans="1:18" s="13" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B88" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="E82" s="13" t="s">
+      <c r="E88" s="13" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="12" t="s">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A89" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="B83" s="24"/>
-      <c r="C83" s="1"/>
-      <c r="D83" s="17"/>
-      <c r="E83" s="1"/>
-    </row>
-    <row r="84" spans="1:5" ht="63" x14ac:dyDescent="0.25">
-      <c r="B84" s="13" t="s">
+      <c r="B89" s="24"/>
+      <c r="C89" s="1"/>
+      <c r="D89" s="17"/>
+      <c r="E89" s="1"/>
+    </row>
+    <row r="90" spans="1:18" ht="63" x14ac:dyDescent="0.25">
+      <c r="B90" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="D84" s="18"/>
-      <c r="E84" s="8" t="s">
+      <c r="D90" s="18"/>
+      <c r="E90" s="8" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="63" x14ac:dyDescent="0.25">
-      <c r="B85" s="13" t="s">
+    <row r="91" spans="1:18" ht="63" x14ac:dyDescent="0.25">
+      <c r="B91" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="D85" s="18"/>
-      <c r="E85" s="8" t="s">
+      <c r="D91" s="18"/>
+      <c r="E91" s="8" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="63" x14ac:dyDescent="0.25">
-      <c r="B86" s="13" t="s">
+    <row r="92" spans="1:18" ht="63" x14ac:dyDescent="0.25">
+      <c r="B92" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="D86" s="18"/>
-      <c r="E86" s="8" t="s">
+      <c r="D92" s="18"/>
+      <c r="E92" s="8" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="63" x14ac:dyDescent="0.25">
-      <c r="B87" s="13" t="s">
+    <row r="93" spans="1:18" ht="63" x14ac:dyDescent="0.25">
+      <c r="B93" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="D87" s="18"/>
-      <c r="E87" s="8" t="s">
+      <c r="D93" s="18"/>
+      <c r="E93" s="8" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="63" x14ac:dyDescent="0.25">
-      <c r="B88" s="13" t="s">
+    <row r="94" spans="1:18" ht="63" x14ac:dyDescent="0.25">
+      <c r="B94" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="D88" s="18"/>
-      <c r="E88" s="8" t="s">
+      <c r="D94" s="18"/>
+      <c r="E94" s="8" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="63" x14ac:dyDescent="0.25">
-      <c r="B89" s="13" t="s">
+    <row r="95" spans="1:18" ht="63" x14ac:dyDescent="0.25">
+      <c r="B95" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="D89" s="18"/>
-      <c r="E89" s="8" t="s">
+      <c r="D95" s="18"/>
+      <c r="E95" s="8" t="s">
         <v>145</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added "sentence date”, "sentence duration, “parole and “incarcerated indicators” to the Custody Search and Query results.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Custody_Query_Results/artifacts/service_model/information_model/IEPD/documentation/impl/CustodyQueryResults.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Custody_Query_Results/artifacts/service_model/information_model/IEPD/documentation/impl/CustodyQueryResults.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2070" yWindow="465" windowWidth="20580" windowHeight="9870" tabRatio="500"/>
+    <workbookView xWindow="11820" yWindow="1520" windowWidth="20580" windowHeight="15340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Custody Query Results Mappin" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="222">
   <si>
     <t>Race</t>
   </si>
@@ -661,6 +661,30 @@
   </si>
   <si>
     <t>/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/nc:Identity[@structures:id=/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/nc:PersonAliasIdentityAssociation/nc:Identity/@structures:ref]/nc:IdentityPersonRepresentation/j:PersonSexCode</t>
+  </si>
+  <si>
+    <t>Charge SentenceDate</t>
+  </si>
+  <si>
+    <t>Charge Sentence Duration</t>
+  </si>
+  <si>
+    <t>/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/j:Charge[@structures:id=/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/j:Arrest/j:ArrestCharge/@structures:ref]/j:ChargeSentence/nc:ActivityDate/nc:Date</t>
+  </si>
+  <si>
+    <t>/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/j:Charge[@structures:id=/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/j:Arrest/j:ArrestCharge/@structures:ref]/j:ChargeSentence/j:SentenceTerm/j:TermDuration</t>
+  </si>
+  <si>
+    <t>Person Incarcerated Indicator</t>
+  </si>
+  <si>
+    <t>Person Probationer Indicator</t>
+  </si>
+  <si>
+    <t>/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/nc:Person[@structures:id=/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/j:PersonAugmentation/j:PersonProbationerIndicator</t>
+  </si>
+  <si>
+    <t>/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/nc:Person[@structures:id=/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/cq-res-ext:PersonIncarceratedIndicator</t>
   </si>
 </sst>
 </file>
@@ -794,7 +818,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="784">
+  <cellStyleXfs count="796">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1503,6 +1527,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1679,7 +1715,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="784">
+  <cellStyles count="796">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2071,6 +2107,12 @@
     <cellStyle name="Followed Hyperlink" xfId="779" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="781" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="783" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="785" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="787" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="789" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="791" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="793" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="795" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2462,6 +2504,12 @@
     <cellStyle name="Hyperlink" xfId="778" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="780" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="782" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="784" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="786" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="788" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="790" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="792" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="794" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="707" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2797,24 +2845,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R95"/>
+  <dimension ref="A1:R99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A42" sqref="A42"/>
+      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A38" sqref="A38:XFD39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="23.5" style="2" customWidth="1"/>
-    <col min="2" max="2" width="26.625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="27.625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="12.875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="84.875" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="10.875" style="2"/>
+    <col min="2" max="2" width="26.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="84.83203125" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="20" customFormat="1">
       <c r="A1" s="32" t="s">
         <v>147</v>
       </c>
@@ -2826,7 +2874,7 @@
       <c r="G1" s="21"/>
       <c r="H1" s="21"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="19" t="s">
         <v>3</v>
       </c>
@@ -2843,7 +2891,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="12" t="s">
         <v>5</v>
       </c>
@@ -2852,7 +2900,7 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="31.5">
       <c r="A4" s="14"/>
       <c r="B4" s="14" t="s">
         <v>8</v>
@@ -2865,7 +2913,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="14"/>
       <c r="B5" s="3" t="s">
         <v>6</v>
@@ -2878,7 +2926,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="12" t="s">
         <v>24</v>
       </c>
@@ -2887,7 +2935,7 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="B7" s="2" t="s">
         <v>25</v>
       </c>
@@ -2898,7 +2946,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="B8" s="2" t="s">
         <v>27</v>
       </c>
@@ -2909,7 +2957,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="12" t="s">
         <v>102</v>
       </c>
@@ -2918,7 +2966,7 @@
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="63">
       <c r="A10" s="14"/>
       <c r="B10" s="8" t="s">
         <v>103</v>
@@ -2929,7 +2977,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="12" t="s">
         <v>55</v>
       </c>
@@ -2938,7 +2986,7 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:8" s="5" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="5" customFormat="1" ht="63">
       <c r="A12" s="15"/>
       <c r="B12" s="3" t="s">
         <v>126</v>
@@ -2949,7 +2997,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="5" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="5" customFormat="1" ht="47.25">
       <c r="A13" s="15"/>
       <c r="B13" s="3" t="s">
         <v>202</v>
@@ -2960,7 +3008,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="5" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" s="5" customFormat="1" ht="47.25">
       <c r="A14" s="15"/>
       <c r="B14" s="3" t="s">
         <v>203</v>
@@ -2971,7 +3019,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="5" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" s="5" customFormat="1" ht="47.25">
       <c r="A15" s="15"/>
       <c r="B15" s="3" t="s">
         <v>205</v>
@@ -2982,7 +3030,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="5" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" s="5" customFormat="1" ht="47.25">
       <c r="A16" s="15"/>
       <c r="B16" s="3" t="s">
         <v>204</v>
@@ -2993,7 +3041,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="5" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" s="5" customFormat="1" ht="63">
       <c r="A17" s="15"/>
       <c r="B17" s="3" t="s">
         <v>127</v>
@@ -3004,7 +3052,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="5" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" s="5" customFormat="1" ht="63">
       <c r="A18" s="15"/>
       <c r="B18" s="3" t="s">
         <v>128</v>
@@ -3015,7 +3063,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="5" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" s="5" customFormat="1" ht="63">
       <c r="A19" s="15"/>
       <c r="B19" s="3" t="s">
         <v>129</v>
@@ -3026,7 +3074,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="63">
       <c r="A20" s="14"/>
       <c r="B20" s="14" t="s">
         <v>13</v>
@@ -3039,7 +3087,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="47.25">
       <c r="A21" s="8"/>
       <c r="B21" s="8" t="s">
         <v>2</v>
@@ -3052,7 +3100,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="47.25">
       <c r="A22" s="8"/>
       <c r="B22" s="8" t="s">
         <v>0</v>
@@ -3065,7 +3113,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="63">
       <c r="A23" s="14"/>
       <c r="B23" s="14" t="s">
         <v>22</v>
@@ -3078,7 +3126,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="63">
       <c r="A24" s="10"/>
       <c r="B24" s="4" t="s">
         <v>63</v>
@@ -3091,7 +3139,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="63">
       <c r="A25" s="10"/>
       <c r="B25" s="4" t="s">
         <v>109</v>
@@ -3104,7 +3152,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="63">
       <c r="A26" s="10"/>
       <c r="B26" s="4" t="s">
         <v>114</v>
@@ -3117,7 +3165,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="63">
       <c r="A27" s="10"/>
       <c r="B27" s="4" t="s">
         <v>113</v>
@@ -3130,7 +3178,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="63">
       <c r="A28" s="3"/>
       <c r="B28" s="3" t="s">
         <v>65</v>
@@ -3143,7 +3191,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="63">
       <c r="A29" s="3"/>
       <c r="B29" s="4" t="s">
         <v>67</v>
@@ -3156,7 +3204,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="63">
       <c r="A30" s="3"/>
       <c r="B30" s="3" t="s">
         <v>69</v>
@@ -3169,7 +3217,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="47.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4" t="s">
         <v>1</v>
@@ -3182,7 +3230,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="47.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4" t="s">
         <v>71</v>
@@ -3195,7 +3243,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="63" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" ht="63">
       <c r="A33" s="4"/>
       <c r="B33" s="4" t="s">
         <v>104</v>
@@ -3206,7 +3254,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="34" spans="1:13" s="13" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" s="13" customFormat="1" ht="78.75">
       <c r="A34" s="4"/>
       <c r="B34" s="4" t="s">
         <v>190</v>
@@ -3227,7 +3275,7 @@
       <c r="L34" s="6"/>
       <c r="M34" s="6"/>
     </row>
-    <row r="35" spans="1:13" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" s="13" customFormat="1" ht="63">
       <c r="A35" s="4"/>
       <c r="B35" s="4" t="s">
         <v>192</v>
@@ -3246,7 +3294,7 @@
       <c r="L35" s="6"/>
       <c r="M35" s="6"/>
     </row>
-    <row r="36" spans="1:13" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" s="13" customFormat="1" ht="63">
       <c r="A36" s="4"/>
       <c r="B36" s="4" t="s">
         <v>197</v>
@@ -3265,7 +3313,7 @@
       <c r="L36" s="6"/>
       <c r="M36" s="6"/>
     </row>
-    <row r="37" spans="1:13" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" s="13" customFormat="1" ht="63">
       <c r="A37" s="4"/>
       <c r="B37" s="4" t="s">
         <v>193</v>
@@ -3284,575 +3332,541 @@
       <c r="L37" s="6"/>
       <c r="M37" s="6"/>
     </row>
-    <row r="38" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="30" t="s">
+    <row r="38" spans="1:13" s="13" customFormat="1" ht="60">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="C38" s="4"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="F38" s="27"/>
+      <c r="G38" s="28"/>
+      <c r="H38" s="28"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="6"/>
+      <c r="K38" s="6"/>
+      <c r="L38" s="6"/>
+      <c r="M38" s="6"/>
+    </row>
+    <row r="39" spans="1:13" s="13" customFormat="1" ht="60">
+      <c r="A39" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="C39" s="4"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="F39" s="27"/>
+      <c r="G39" s="28"/>
+      <c r="H39" s="28"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="6"/>
+      <c r="K39" s="6"/>
+      <c r="L39" s="6"/>
+      <c r="M39" s="6"/>
+    </row>
+    <row r="40" spans="1:13" s="13" customFormat="1">
+      <c r="A40" s="30" t="s">
         <v>208</v>
       </c>
-      <c r="B38" s="24"/>
-      <c r="C38" s="24"/>
-      <c r="D38" s="24"/>
-      <c r="E38" s="24"/>
-    </row>
-    <row r="39" spans="1:13" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
-      <c r="A39" s="8"/>
-      <c r="B39" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="D39" s="8"/>
-      <c r="E39" s="31" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
-      <c r="A40" s="8"/>
-      <c r="B40" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="D40" s="8"/>
-      <c r="E40" s="31" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="B40" s="24"/>
+      <c r="C40" s="24"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="24"/>
+    </row>
+    <row r="41" spans="1:13" s="13" customFormat="1" ht="63">
       <c r="A41" s="8"/>
       <c r="B41" s="8" t="s">
-        <v>67</v>
+        <v>13</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="D41" s="8"/>
       <c r="E41" s="31" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" s="13" customFormat="1" ht="63">
       <c r="A42" s="8"/>
       <c r="B42" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="D42" s="8"/>
       <c r="E42" s="31" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" s="13" customFormat="1" ht="63">
       <c r="A43" s="8"/>
       <c r="B43" s="8" t="s">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D43" s="8"/>
       <c r="E43" s="31" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" s="13" customFormat="1" ht="63">
+      <c r="A44" s="8"/>
+      <c r="B44" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D44" s="8"/>
+      <c r="E44" s="31" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" s="13" customFormat="1" ht="63">
+      <c r="A45" s="8"/>
+      <c r="B45" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D45" s="8"/>
+      <c r="E45" s="31" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" s="12" t="s">
+    <row r="46" spans="1:13">
+      <c r="A46" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-    </row>
-    <row r="45" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B45" s="4" t="s">
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+    </row>
+    <row r="47" spans="1:13" ht="47.25">
+      <c r="B47" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C47" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E45" s="9" t="s">
+      <c r="E47" s="9" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B46" s="3" t="s">
+    <row r="48" spans="1:13" ht="47.25">
+      <c r="B48" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C48" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E46" s="9" t="s">
+      <c r="E48" s="9" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="5"/>
-      <c r="B47" s="5" t="s">
+    <row r="49" spans="1:5" ht="78.75">
+      <c r="A49" s="5"/>
+      <c r="B49" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C47" s="5" t="s">
+      <c r="C49" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D47" s="5"/>
-      <c r="E47" s="7" t="s">
+      <c r="D49" s="5"/>
+      <c r="E49" s="7" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A48" s="12" t="s">
+    <row r="50" spans="1:5">
+      <c r="A50" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-    </row>
-    <row r="49" spans="1:5" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
-      <c r="A49" s="29"/>
-      <c r="B49" s="4" t="s">
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+    </row>
+    <row r="51" spans="1:5" s="13" customFormat="1" ht="63">
+      <c r="A51" s="29"/>
+      <c r="B51" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="14" t="s">
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="14" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="63" x14ac:dyDescent="0.25">
-      <c r="A50" s="16"/>
-      <c r="B50" s="8" t="s">
+    <row r="52" spans="1:5" ht="63">
+      <c r="A52" s="16"/>
+      <c r="B52" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="C50" s="14" t="s">
+      <c r="C52" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14" t="s">
+      <c r="D52" s="14"/>
+      <c r="E52" s="14" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A51" s="14"/>
-      <c r="B51" s="8" t="s">
+    <row r="53" spans="1:5" ht="47.25">
+      <c r="A53" s="14"/>
+      <c r="B53" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C51" s="8" t="s">
+      <c r="C53" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D51" s="8"/>
-      <c r="E51" s="14" t="s">
+      <c r="D53" s="8"/>
+      <c r="E53" s="14" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="63" x14ac:dyDescent="0.25">
-      <c r="A52" s="14"/>
-      <c r="B52" s="8" t="s">
+    <row r="54" spans="1:5" ht="63">
+      <c r="A54" s="14"/>
+      <c r="B54" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="C52" s="8" t="s">
+      <c r="C54" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="D52" s="8"/>
-      <c r="E52" s="14" t="s">
+      <c r="D54" s="8"/>
+      <c r="E54" s="14" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="63" x14ac:dyDescent="0.25">
-      <c r="B53" s="4" t="s">
+    <row r="55" spans="1:5" ht="63">
+      <c r="B55" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C55" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E53" s="14" t="s">
+      <c r="E55" s="14" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="12" t="s">
+    <row r="56" spans="1:5">
+      <c r="A56" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-    </row>
-    <row r="55" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A55" s="5"/>
-      <c r="B55" s="5" t="s">
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+    </row>
+    <row r="57" spans="1:5" ht="47.25">
+      <c r="A57" s="5"/>
+      <c r="B57" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
-      <c r="E55" s="3" t="s">
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="3" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A56" s="5"/>
-      <c r="B56" s="4" t="s">
+    <row r="58" spans="1:5" ht="47.25">
+      <c r="A58" s="5"/>
+      <c r="B58" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C56" s="5" t="s">
+      <c r="C58" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D56" s="5"/>
-      <c r="E56" s="3" t="s">
+      <c r="D58" s="5"/>
+      <c r="E58" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="12" t="s">
+    <row r="59" spans="1:5">
+      <c r="A59" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
-    </row>
-    <row r="58" spans="1:5" ht="63" x14ac:dyDescent="0.25">
-      <c r="B58" s="4" t="s">
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+    </row>
+    <row r="60" spans="1:5" ht="63">
+      <c r="B60" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C60" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E58" s="2" t="s">
+      <c r="E60" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B59" s="4" t="s">
+    <row r="61" spans="1:5" ht="47.25">
+      <c r="B61" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="C61" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E59" s="9" t="s">
+      <c r="E61" s="9" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="63" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
+    <row r="62" spans="1:5" ht="63">
+      <c r="A62" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B62" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C62" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E60" s="2" t="s">
+      <c r="E62" s="2" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="63" x14ac:dyDescent="0.25">
-      <c r="B61" s="4" t="s">
+    <row r="63" spans="1:5" ht="63">
+      <c r="B63" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="C63" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E61" s="2" t="s">
+      <c r="E63" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="62" spans="1:5" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
-      <c r="A62" s="8"/>
-      <c r="B62" s="8" t="s">
+    <row r="64" spans="1:5" s="13" customFormat="1" ht="63">
+      <c r="A64" s="8"/>
+      <c r="B64" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="C62" s="13" t="s">
+      <c r="C64" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="E62" s="2" t="s">
+      <c r="E64" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="63" spans="1:5" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
-      <c r="A63" s="8"/>
-      <c r="B63" s="13" t="s">
+    <row r="65" spans="1:5" s="13" customFormat="1" ht="63">
+      <c r="A65" s="8"/>
+      <c r="B65" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="C63" s="13" t="s">
+      <c r="C65" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="E63" s="2" t="s">
+      <c r="E65" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="63" x14ac:dyDescent="0.25">
-      <c r="A64" s="5"/>
-      <c r="B64" s="6" t="s">
+    <row r="66" spans="1:5" ht="63">
+      <c r="A66" s="5"/>
+      <c r="B66" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C64" s="5" t="s">
+      <c r="C66" s="5" t="s">
         <v>48</v>
-      </c>
-      <c r="D64" s="5"/>
-      <c r="E64" s="5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="65" spans="1:18" ht="63" x14ac:dyDescent="0.25">
-      <c r="A65" s="5"/>
-      <c r="B65" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="C65" s="5"/>
-      <c r="D65" s="5"/>
-      <c r="E65" s="5" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="66" spans="1:18" ht="63" x14ac:dyDescent="0.25">
-      <c r="A66" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B66" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>50</v>
       </c>
       <c r="D66" s="5"/>
       <c r="E66" s="5" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="67" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A67" s="5" t="s">
-        <v>38</v>
-      </c>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="63">
+      <c r="A67" s="5"/>
       <c r="B67" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C67" s="5" t="s">
-        <v>52</v>
-      </c>
+        <v>187</v>
+      </c>
+      <c r="C67" s="5"/>
       <c r="D67" s="5"/>
       <c r="E67" s="5" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="63">
+      <c r="A68" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D68" s="5"/>
+      <c r="E68" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="47.25">
+      <c r="A69" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D69" s="5"/>
+      <c r="E69" s="5" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A68" s="12" t="s">
+    <row r="70" spans="1:5">
+      <c r="A70" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B68" s="24"/>
-      <c r="C68" s="1"/>
-      <c r="D68" s="1"/>
-      <c r="E68" s="1"/>
-    </row>
-    <row r="69" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B69" s="4" t="s">
+      <c r="B70" s="24"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+    </row>
+    <row r="71" spans="1:5" ht="47.25">
+      <c r="B71" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="C71" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E69" s="14" t="s">
+      <c r="E71" s="14" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="70" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B70" s="4" t="s">
+    <row r="72" spans="1:5" ht="47.25">
+      <c r="B72" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="E70" s="14" t="s">
+      <c r="E72" s="14" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="71" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B71" s="4" t="s">
+    <row r="73" spans="1:5" ht="47.25">
+      <c r="B73" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="C73" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E71" s="14" t="s">
+      <c r="E73" s="14" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="72" spans="1:18" ht="63" x14ac:dyDescent="0.25">
-      <c r="B72" s="4" t="s">
+    <row r="74" spans="1:5" ht="63">
+      <c r="B74" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="C74" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E72" s="14" t="s">
+      <c r="E74" s="14" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="73" spans="1:18" ht="63" x14ac:dyDescent="0.25">
-      <c r="B73" s="4" t="s">
+    <row r="75" spans="1:5" ht="63">
+      <c r="B75" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C73" s="2" t="s">
+      <c r="C75" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="E73" s="14" t="s">
+      <c r="E75" s="14" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="74" spans="1:18" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A74" s="5"/>
-      <c r="B74" s="6" t="s">
+    <row r="76" spans="1:5" ht="105">
+      <c r="A76" s="5"/>
+      <c r="B76" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C74" s="6" t="s">
+      <c r="C76" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D74" s="6"/>
-      <c r="E74" s="5" t="s">
+      <c r="D76" s="6"/>
+      <c r="E76" s="5" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="75" spans="1:18" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="5"/>
-      <c r="B75" s="6" t="s">
+    <row r="77" spans="1:5" ht="60" customHeight="1">
+      <c r="A77" s="5"/>
+      <c r="B77" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C75" s="5"/>
-      <c r="D75" s="5"/>
-      <c r="E75" s="14" t="s">
+      <c r="C77" s="5"/>
+      <c r="D77" s="5"/>
+      <c r="E77" s="14" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="76" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A76" s="5" t="s">
+    <row r="78" spans="1:5" ht="60" customHeight="1">
+      <c r="A78" s="5"/>
+      <c r="B78" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="C78" s="5"/>
+      <c r="D78" s="5"/>
+      <c r="E78" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="60" customHeight="1">
+      <c r="A79" s="5"/>
+      <c r="B79" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="C79" s="5"/>
+      <c r="D79" s="5"/>
+      <c r="E79" s="14" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="47.25">
+      <c r="A80" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="B80" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C76" s="5" t="s">
+      <c r="C80" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D76" s="5"/>
-      <c r="E76" s="5" t="s">
+      <c r="D80" s="5"/>
+      <c r="E80" s="5" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A77" s="12" t="s">
+    <row r="81" spans="1:18">
+      <c r="A81" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B77" s="24"/>
-      <c r="C77" s="1"/>
-      <c r="D77" s="1"/>
-      <c r="E77" s="1"/>
-    </row>
-    <row r="78" spans="1:18" s="13" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A78" s="6"/>
-      <c r="B78" s="25" t="s">
-        <v>170</v>
-      </c>
-      <c r="C78" s="6"/>
-      <c r="D78" s="22"/>
-      <c r="E78" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="F78" s="23"/>
-      <c r="G78" s="23"/>
-      <c r="H78" s="23"/>
-      <c r="I78" s="4"/>
-      <c r="J78" s="6"/>
-      <c r="K78" s="6"/>
-      <c r="L78" s="6"/>
-      <c r="M78" s="6"/>
-      <c r="N78" s="6"/>
-      <c r="O78" s="6"/>
-      <c r="P78" s="6"/>
-      <c r="Q78" s="6"/>
-      <c r="R78" s="6"/>
-    </row>
-    <row r="79" spans="1:18" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
-      <c r="A79" s="6"/>
-      <c r="B79" s="25" t="s">
-        <v>171</v>
-      </c>
-      <c r="C79" s="6"/>
-      <c r="D79" s="22"/>
-      <c r="E79" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="F79" s="23"/>
-      <c r="G79" s="23"/>
-      <c r="H79" s="23"/>
-      <c r="I79" s="4"/>
-      <c r="J79" s="6"/>
-      <c r="K79" s="6"/>
-      <c r="L79" s="6"/>
-      <c r="M79" s="6"/>
-      <c r="N79" s="6"/>
-      <c r="O79" s="6"/>
-      <c r="P79" s="6"/>
-      <c r="Q79" s="6"/>
-      <c r="R79" s="6"/>
-    </row>
-    <row r="80" spans="1:18" s="13" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A80" s="6"/>
-      <c r="B80" s="25" t="s">
-        <v>172</v>
-      </c>
-      <c r="C80" s="6"/>
-      <c r="D80" s="22"/>
-      <c r="E80" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="F80" s="23"/>
-      <c r="G80" s="23"/>
-      <c r="H80" s="23"/>
-      <c r="I80" s="4"/>
-      <c r="J80" s="6"/>
-      <c r="K80" s="6"/>
-      <c r="L80" s="6"/>
-      <c r="M80" s="6"/>
-      <c r="N80" s="6"/>
-      <c r="O80" s="6"/>
-      <c r="P80" s="6"/>
-      <c r="Q80" s="6"/>
-      <c r="R80" s="6"/>
-    </row>
-    <row r="81" spans="1:18" s="13" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A81" s="6"/>
-      <c r="B81" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="C81" s="6"/>
-      <c r="D81" s="22"/>
-      <c r="E81" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="F81" s="23"/>
-      <c r="G81" s="23"/>
-      <c r="H81" s="23"/>
-      <c r="I81" s="4"/>
-      <c r="J81" s="6"/>
-      <c r="K81" s="6"/>
-      <c r="L81" s="6"/>
-      <c r="M81" s="6"/>
-      <c r="N81" s="6"/>
-      <c r="O81" s="6"/>
-      <c r="P81" s="6"/>
-      <c r="Q81" s="6"/>
-      <c r="R81" s="6"/>
-    </row>
-    <row r="82" spans="1:18" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="B81" s="24"/>
+      <c r="C81" s="1"/>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1"/>
+    </row>
+    <row r="82" spans="1:18" s="13" customFormat="1" ht="47.25">
       <c r="A82" s="6"/>
       <c r="B82" s="25" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C82" s="6"/>
       <c r="D82" s="22"/>
       <c r="E82" s="3" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="F82" s="23"/>
       <c r="G82" s="23"/>
@@ -3868,15 +3882,15 @@
       <c r="Q82" s="6"/>
       <c r="R82" s="6"/>
     </row>
-    <row r="83" spans="1:18" s="13" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:18" s="13" customFormat="1" ht="63">
       <c r="A83" s="6"/>
       <c r="B83" s="25" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C83" s="6"/>
       <c r="D83" s="22"/>
       <c r="E83" s="3" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="F83" s="23"/>
       <c r="G83" s="23"/>
@@ -3892,118 +3906,214 @@
       <c r="Q83" s="6"/>
       <c r="R83" s="6"/>
     </row>
-    <row r="84" spans="1:18" ht="63" x14ac:dyDescent="0.25">
-      <c r="A84" s="5"/>
-      <c r="B84" s="6" t="s">
+    <row r="84" spans="1:18" s="13" customFormat="1" ht="47.25">
+      <c r="A84" s="6"/>
+      <c r="B84" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="C84" s="6"/>
+      <c r="D84" s="22"/>
+      <c r="E84" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="F84" s="23"/>
+      <c r="G84" s="23"/>
+      <c r="H84" s="23"/>
+      <c r="I84" s="4"/>
+      <c r="J84" s="6"/>
+      <c r="K84" s="6"/>
+      <c r="L84" s="6"/>
+      <c r="M84" s="6"/>
+      <c r="N84" s="6"/>
+      <c r="O84" s="6"/>
+      <c r="P84" s="6"/>
+      <c r="Q84" s="6"/>
+      <c r="R84" s="6"/>
+    </row>
+    <row r="85" spans="1:18" s="13" customFormat="1" ht="47.25">
+      <c r="A85" s="6"/>
+      <c r="B85" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="C85" s="6"/>
+      <c r="D85" s="22"/>
+      <c r="E85" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F85" s="23"/>
+      <c r="G85" s="23"/>
+      <c r="H85" s="23"/>
+      <c r="I85" s="4"/>
+      <c r="J85" s="6"/>
+      <c r="K85" s="6"/>
+      <c r="L85" s="6"/>
+      <c r="M85" s="6"/>
+      <c r="N85" s="6"/>
+      <c r="O85" s="6"/>
+      <c r="P85" s="6"/>
+      <c r="Q85" s="6"/>
+      <c r="R85" s="6"/>
+    </row>
+    <row r="86" spans="1:18" s="13" customFormat="1" ht="63">
+      <c r="A86" s="6"/>
+      <c r="B86" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="C86" s="6"/>
+      <c r="D86" s="22"/>
+      <c r="E86" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="F86" s="23"/>
+      <c r="G86" s="23"/>
+      <c r="H86" s="23"/>
+      <c r="I86" s="4"/>
+      <c r="J86" s="6"/>
+      <c r="K86" s="6"/>
+      <c r="L86" s="6"/>
+      <c r="M86" s="6"/>
+      <c r="N86" s="6"/>
+      <c r="O86" s="6"/>
+      <c r="P86" s="6"/>
+      <c r="Q86" s="6"/>
+      <c r="R86" s="6"/>
+    </row>
+    <row r="87" spans="1:18" s="13" customFormat="1" ht="47.25">
+      <c r="A87" s="6"/>
+      <c r="B87" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="C87" s="6"/>
+      <c r="D87" s="22"/>
+      <c r="E87" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="F87" s="23"/>
+      <c r="G87" s="23"/>
+      <c r="H87" s="23"/>
+      <c r="I87" s="4"/>
+      <c r="J87" s="6"/>
+      <c r="K87" s="6"/>
+      <c r="L87" s="6"/>
+      <c r="M87" s="6"/>
+      <c r="N87" s="6"/>
+      <c r="O87" s="6"/>
+      <c r="P87" s="6"/>
+      <c r="Q87" s="6"/>
+      <c r="R87" s="6"/>
+    </row>
+    <row r="88" spans="1:18" ht="63">
+      <c r="A88" s="5"/>
+      <c r="B88" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="C84" s="6"/>
-      <c r="D84" s="11"/>
-      <c r="E84" s="3" t="s">
+      <c r="C88" s="6"/>
+      <c r="D88" s="11"/>
+      <c r="E88" s="3" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="85" spans="1:18" ht="63" x14ac:dyDescent="0.25">
-      <c r="A85" s="5"/>
-      <c r="B85" s="6" t="s">
+    <row r="89" spans="1:18" ht="63">
+      <c r="A89" s="5"/>
+      <c r="B89" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="C85" s="6"/>
-      <c r="D85" s="11"/>
-      <c r="E85" s="3" t="s">
+      <c r="C89" s="6"/>
+      <c r="D89" s="11"/>
+      <c r="E89" s="3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="86" spans="1:18" ht="63" x14ac:dyDescent="0.25">
-      <c r="A86" s="5"/>
-      <c r="B86" s="6" t="s">
+    <row r="90" spans="1:18" ht="63">
+      <c r="A90" s="5"/>
+      <c r="B90" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C86" s="5" t="s">
+      <c r="C90" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D86" s="5"/>
-      <c r="E86" s="5" t="s">
+      <c r="D90" s="5"/>
+      <c r="E90" s="5" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A87" s="12" t="s">
+    <row r="91" spans="1:18">
+      <c r="A91" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="B87" s="24"/>
-      <c r="C87" s="1"/>
-      <c r="D87" s="1"/>
-      <c r="E87" s="1"/>
-    </row>
-    <row r="88" spans="1:18" s="13" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B88" s="4" t="s">
+      <c r="B91" s="24"/>
+      <c r="C91" s="1"/>
+      <c r="D91" s="1"/>
+      <c r="E91" s="1"/>
+    </row>
+    <row r="92" spans="1:18" s="13" customFormat="1" ht="47.25">
+      <c r="B92" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="E88" s="13" t="s">
+      <c r="E92" s="13" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A89" s="12" t="s">
+    <row r="93" spans="1:18">
+      <c r="A93" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="B89" s="24"/>
-      <c r="C89" s="1"/>
-      <c r="D89" s="17"/>
-      <c r="E89" s="1"/>
-    </row>
-    <row r="90" spans="1:18" ht="63" x14ac:dyDescent="0.25">
-      <c r="B90" s="13" t="s">
+      <c r="B93" s="24"/>
+      <c r="C93" s="1"/>
+      <c r="D93" s="17"/>
+      <c r="E93" s="1"/>
+    </row>
+    <row r="94" spans="1:18" ht="63">
+      <c r="B94" s="13" t="s">
         <v>137</v>
-      </c>
-      <c r="D90" s="18"/>
-      <c r="E90" s="8" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="91" spans="1:18" ht="63" x14ac:dyDescent="0.25">
-      <c r="B91" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="D91" s="18"/>
-      <c r="E91" s="8" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="92" spans="1:18" ht="63" x14ac:dyDescent="0.25">
-      <c r="B92" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="D92" s="18"/>
-      <c r="E92" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="93" spans="1:18" ht="63" x14ac:dyDescent="0.25">
-      <c r="B93" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="D93" s="18"/>
-      <c r="E93" s="8" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="94" spans="1:18" ht="63" x14ac:dyDescent="0.25">
-      <c r="B94" s="13" t="s">
-        <v>141</v>
       </c>
       <c r="D94" s="18"/>
       <c r="E94" s="8" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="95" spans="1:18" ht="63" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="95" spans="1:18" ht="63">
       <c r="B95" s="13" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D95" s="18"/>
       <c r="E95" s="8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18" ht="63">
+      <c r="B96" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="D96" s="18"/>
+      <c r="E96" s="8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="97" spans="2:5" ht="63">
+      <c r="B97" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="D97" s="18"/>
+      <c r="E97" s="8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="98" spans="2:5" ht="63">
+      <c r="B98" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="D98" s="18"/>
+      <c r="E98" s="8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="99" spans="2:5" ht="63">
+      <c r="B99" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="D99" s="18"/>
+      <c r="E99" s="8" t="s">
         <v>145</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added SupervisionCondition to the XML sample file.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Custody_Query_Results/artifacts/service_model/information_model/IEPD/documentation/impl/CustodyQueryResults.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Custody_Query_Results/artifacts/service_model/information_model/IEPD/documentation/impl/CustodyQueryResults.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11820" yWindow="1520" windowWidth="20580" windowHeight="15340" tabRatio="500"/>
+    <workbookView xWindow="-23860" yWindow="1180" windowWidth="20580" windowHeight="15340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Custody Query Results Mappin" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="224">
   <si>
     <t>Race</t>
   </si>
@@ -685,6 +685,12 @@
   </si>
   <si>
     <t>/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/nc:Person[@structures:id=/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/cq-res-ext:PersonIncarceratedIndicator</t>
+  </si>
+  <si>
+    <t>Supervision Condition</t>
+  </si>
+  <si>
+    <t>/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/j:Detention[@structures:id=/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/j:ActivityCaseAssociation/nc:Activity/@structures:ref]/j:SupervisionAugmentation/j:SupervisionCondition/nc:ActivityDescriptionText</t>
   </si>
 </sst>
 </file>
@@ -818,7 +824,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="796">
+  <cellStyleXfs count="798">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1527,6 +1533,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1715,7 +1723,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="796">
+  <cellStyles count="798">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2113,6 +2121,7 @@
     <cellStyle name="Followed Hyperlink" xfId="791" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="793" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="795" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="797" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2510,6 +2519,7 @@
     <cellStyle name="Hyperlink" xfId="790" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="792" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="794" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="796" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="707" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2845,11 +2855,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R99"/>
+  <dimension ref="A1:R100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A38" sqref="A38:XFD39"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2900,7 +2910,7 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:8" ht="31.5">
+    <row r="4" spans="1:8" ht="30">
       <c r="A4" s="14"/>
       <c r="B4" s="14" t="s">
         <v>8</v>
@@ -2966,7 +2976,7 @@
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:8" ht="63">
+    <row r="10" spans="1:8" ht="60">
       <c r="A10" s="14"/>
       <c r="B10" s="8" t="s">
         <v>103</v>
@@ -2986,7 +2996,7 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:8" s="5" customFormat="1" ht="63">
+    <row r="12" spans="1:8" s="5" customFormat="1" ht="60">
       <c r="A12" s="15"/>
       <c r="B12" s="3" t="s">
         <v>126</v>
@@ -2997,7 +3007,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="5" customFormat="1" ht="47.25">
+    <row r="13" spans="1:8" s="5" customFormat="1" ht="45">
       <c r="A13" s="15"/>
       <c r="B13" s="3" t="s">
         <v>202</v>
@@ -3008,7 +3018,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="5" customFormat="1" ht="47.25">
+    <row r="14" spans="1:8" s="5" customFormat="1" ht="45">
       <c r="A14" s="15"/>
       <c r="B14" s="3" t="s">
         <v>203</v>
@@ -3019,7 +3029,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="5" customFormat="1" ht="47.25">
+    <row r="15" spans="1:8" s="5" customFormat="1" ht="45">
       <c r="A15" s="15"/>
       <c r="B15" s="3" t="s">
         <v>205</v>
@@ -3030,7 +3040,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="5" customFormat="1" ht="47.25">
+    <row r="16" spans="1:8" s="5" customFormat="1" ht="45">
       <c r="A16" s="15"/>
       <c r="B16" s="3" t="s">
         <v>204</v>
@@ -3041,7 +3051,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="5" customFormat="1" ht="63">
+    <row r="17" spans="1:5" s="5" customFormat="1" ht="60">
       <c r="A17" s="15"/>
       <c r="B17" s="3" t="s">
         <v>127</v>
@@ -3052,7 +3062,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="5" customFormat="1" ht="63">
+    <row r="18" spans="1:5" s="5" customFormat="1" ht="60">
       <c r="A18" s="15"/>
       <c r="B18" s="3" t="s">
         <v>128</v>
@@ -3063,7 +3073,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="5" customFormat="1" ht="63">
+    <row r="19" spans="1:5" s="5" customFormat="1" ht="60">
       <c r="A19" s="15"/>
       <c r="B19" s="3" t="s">
         <v>129</v>
@@ -3074,7 +3084,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="63">
+    <row r="20" spans="1:5" ht="60">
       <c r="A20" s="14"/>
       <c r="B20" s="14" t="s">
         <v>13</v>
@@ -3087,7 +3097,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="47.25">
+    <row r="21" spans="1:5" ht="45">
       <c r="A21" s="8"/>
       <c r="B21" s="8" t="s">
         <v>2</v>
@@ -3100,7 +3110,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="47.25">
+    <row r="22" spans="1:5" ht="45">
       <c r="A22" s="8"/>
       <c r="B22" s="8" t="s">
         <v>0</v>
@@ -3113,7 +3123,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="63">
+    <row r="23" spans="1:5" ht="60">
       <c r="A23" s="14"/>
       <c r="B23" s="14" t="s">
         <v>22</v>
@@ -3126,7 +3136,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="63">
+    <row r="24" spans="1:5" ht="60">
       <c r="A24" s="10"/>
       <c r="B24" s="4" t="s">
         <v>63</v>
@@ -3139,7 +3149,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="63">
+    <row r="25" spans="1:5" ht="60">
       <c r="A25" s="10"/>
       <c r="B25" s="4" t="s">
         <v>109</v>
@@ -3152,7 +3162,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="63">
+    <row r="26" spans="1:5" ht="60">
       <c r="A26" s="10"/>
       <c r="B26" s="4" t="s">
         <v>114</v>
@@ -3165,7 +3175,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="63">
+    <row r="27" spans="1:5" ht="60">
       <c r="A27" s="10"/>
       <c r="B27" s="4" t="s">
         <v>113</v>
@@ -3178,7 +3188,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="63">
+    <row r="28" spans="1:5" ht="60">
       <c r="A28" s="3"/>
       <c r="B28" s="3" t="s">
         <v>65</v>
@@ -3191,7 +3201,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="63">
+    <row r="29" spans="1:5" ht="60">
       <c r="A29" s="3"/>
       <c r="B29" s="4" t="s">
         <v>67</v>
@@ -3204,7 +3214,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="63">
+    <row r="30" spans="1:5" ht="60">
       <c r="A30" s="3"/>
       <c r="B30" s="3" t="s">
         <v>69</v>
@@ -3217,7 +3227,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="47.25">
+    <row r="31" spans="1:5" ht="45">
       <c r="A31" s="4"/>
       <c r="B31" s="4" t="s">
         <v>1</v>
@@ -3230,7 +3240,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="47.25">
+    <row r="32" spans="1:5" ht="45">
       <c r="A32" s="4"/>
       <c r="B32" s="4" t="s">
         <v>71</v>
@@ -3243,7 +3253,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="63">
+    <row r="33" spans="1:13" ht="60">
       <c r="A33" s="4"/>
       <c r="B33" s="4" t="s">
         <v>104</v>
@@ -3254,7 +3264,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="34" spans="1:13" s="13" customFormat="1" ht="78.75">
+    <row r="34" spans="1:13" s="13" customFormat="1" ht="75">
       <c r="A34" s="4"/>
       <c r="B34" s="4" t="s">
         <v>190</v>
@@ -3275,7 +3285,7 @@
       <c r="L34" s="6"/>
       <c r="M34" s="6"/>
     </row>
-    <row r="35" spans="1:13" s="13" customFormat="1" ht="63">
+    <row r="35" spans="1:13" s="13" customFormat="1" ht="60">
       <c r="A35" s="4"/>
       <c r="B35" s="4" t="s">
         <v>192</v>
@@ -3294,7 +3304,7 @@
       <c r="L35" s="6"/>
       <c r="M35" s="6"/>
     </row>
-    <row r="36" spans="1:13" s="13" customFormat="1" ht="63">
+    <row r="36" spans="1:13" s="13" customFormat="1" ht="60">
       <c r="A36" s="4"/>
       <c r="B36" s="4" t="s">
         <v>197</v>
@@ -3313,7 +3323,7 @@
       <c r="L36" s="6"/>
       <c r="M36" s="6"/>
     </row>
-    <row r="37" spans="1:13" s="13" customFormat="1" ht="63">
+    <row r="37" spans="1:13" s="13" customFormat="1" ht="60">
       <c r="A37" s="4"/>
       <c r="B37" s="4" t="s">
         <v>193</v>
@@ -3381,7 +3391,7 @@
       <c r="D40" s="24"/>
       <c r="E40" s="24"/>
     </row>
-    <row r="41" spans="1:13" s="13" customFormat="1" ht="63">
+    <row r="41" spans="1:13" s="13" customFormat="1" ht="60">
       <c r="A41" s="8"/>
       <c r="B41" s="8" t="s">
         <v>13</v>
@@ -3394,7 +3404,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="42" spans="1:13" s="13" customFormat="1" ht="63">
+    <row r="42" spans="1:13" s="13" customFormat="1" ht="60">
       <c r="A42" s="8"/>
       <c r="B42" s="8" t="s">
         <v>65</v>
@@ -3407,7 +3417,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="43" spans="1:13" s="13" customFormat="1" ht="63">
+    <row r="43" spans="1:13" s="13" customFormat="1" ht="60">
       <c r="A43" s="8"/>
       <c r="B43" s="8" t="s">
         <v>67</v>
@@ -3420,7 +3430,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="44" spans="1:13" s="13" customFormat="1" ht="63">
+    <row r="44" spans="1:13" s="13" customFormat="1" ht="60">
       <c r="A44" s="8"/>
       <c r="B44" s="8" t="s">
         <v>69</v>
@@ -3433,7 +3443,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="45" spans="1:13" s="13" customFormat="1" ht="63">
+    <row r="45" spans="1:13" s="13" customFormat="1" ht="60">
       <c r="A45" s="8"/>
       <c r="B45" s="8" t="s">
         <v>1</v>
@@ -3455,7 +3465,7 @@
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
     </row>
-    <row r="47" spans="1:13" ht="47.25">
+    <row r="47" spans="1:13" ht="45">
       <c r="B47" s="4" t="s">
         <v>17</v>
       </c>
@@ -3466,7 +3476,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="47.25">
+    <row r="48" spans="1:13" ht="45">
       <c r="B48" s="3" t="s">
         <v>18</v>
       </c>
@@ -3477,7 +3487,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="78.75">
+    <row r="49" spans="1:5" ht="75">
       <c r="A49" s="5"/>
       <c r="B49" s="5" t="s">
         <v>36</v>
@@ -3499,7 +3509,7 @@
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
     </row>
-    <row r="51" spans="1:5" s="13" customFormat="1" ht="63">
+    <row r="51" spans="1:5" s="13" customFormat="1" ht="60">
       <c r="A51" s="29"/>
       <c r="B51" s="4" t="s">
         <v>199</v>
@@ -3510,7 +3520,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="63">
+    <row r="52" spans="1:5" ht="60">
       <c r="A52" s="16"/>
       <c r="B52" s="8" t="s">
         <v>200</v>
@@ -3523,7 +3533,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="47.25">
+    <row r="53" spans="1:5" ht="45">
       <c r="A53" s="14"/>
       <c r="B53" s="8" t="s">
         <v>76</v>
@@ -3536,7 +3546,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="63">
+    <row r="54" spans="1:5" ht="60">
       <c r="A54" s="14"/>
       <c r="B54" s="8" t="s">
         <v>184</v>
@@ -3549,7 +3559,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="63">
+    <row r="55" spans="1:5" ht="60">
       <c r="B55" s="4" t="s">
         <v>23</v>
       </c>
@@ -3569,7 +3579,7 @@
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
     </row>
-    <row r="57" spans="1:5" ht="47.25">
+    <row r="57" spans="1:5" ht="45">
       <c r="A57" s="5"/>
       <c r="B57" s="5" t="s">
         <v>33</v>
@@ -3580,7 +3590,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="47.25">
+    <row r="58" spans="1:5" ht="45">
       <c r="A58" s="5"/>
       <c r="B58" s="4" t="s">
         <v>19</v>
@@ -3602,7 +3612,7 @@
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
     </row>
-    <row r="60" spans="1:5" ht="63">
+    <row r="60" spans="1:5" ht="60">
       <c r="B60" s="4" t="s">
         <v>121</v>
       </c>
@@ -3613,7 +3623,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="47.25">
+    <row r="61" spans="1:5" ht="45">
       <c r="B61" s="4" t="s">
         <v>21</v>
       </c>
@@ -3624,7 +3634,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="63">
+    <row r="62" spans="1:5" ht="60">
       <c r="A62" s="2" t="s">
         <v>38</v>
       </c>
@@ -3638,7 +3648,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="63">
+    <row r="63" spans="1:5" ht="60">
       <c r="B63" s="4" t="s">
         <v>20</v>
       </c>
@@ -3649,7 +3659,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="64" spans="1:5" s="13" customFormat="1" ht="63">
+    <row r="64" spans="1:5" s="13" customFormat="1" ht="60">
       <c r="A64" s="8"/>
       <c r="B64" s="8" t="s">
         <v>122</v>
@@ -3661,7 +3671,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="65" spans="1:5" s="13" customFormat="1" ht="63">
+    <row r="65" spans="1:5" s="13" customFormat="1" ht="60">
       <c r="A65" s="8"/>
       <c r="B65" s="13" t="s">
         <v>124</v>
@@ -3673,224 +3683,209 @@
         <v>155</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="63">
-      <c r="A66" s="5"/>
-      <c r="B66" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D66" s="5"/>
-      <c r="E66" s="5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" ht="63">
+    <row r="66" spans="1:5" s="13" customFormat="1" ht="60">
+      <c r="A66" s="8"/>
+      <c r="B66" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="60">
       <c r="A67" s="5"/>
       <c r="B67" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="C67" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="D67" s="5"/>
       <c r="E67" s="5" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="63">
-      <c r="A68" s="5" t="s">
-        <v>38</v>
-      </c>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="60">
+      <c r="A68" s="5"/>
       <c r="B68" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>50</v>
-      </c>
+        <v>187</v>
+      </c>
+      <c r="C68" s="5"/>
       <c r="D68" s="5"/>
       <c r="E68" s="5" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" ht="47.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="60">
       <c r="A69" s="5" t="s">
         <v>38</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D69" s="5"/>
       <c r="E69" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="45">
+      <c r="A70" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D70" s="5"/>
+      <c r="E70" s="5" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
-      <c r="A70" s="12" t="s">
+    <row r="71" spans="1:5">
+      <c r="A71" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B70" s="24"/>
-      <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
-    </row>
-    <row r="71" spans="1:5" ht="47.25">
-      <c r="B71" s="4" t="s">
+      <c r="B71" s="24"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+    </row>
+    <row r="72" spans="1:5" ht="45">
+      <c r="B72" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="C72" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E71" s="14" t="s">
+      <c r="E72" s="14" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="47.25">
-      <c r="B72" s="4" t="s">
+    <row r="73" spans="1:5" ht="45">
+      <c r="B73" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="E72" s="14" t="s">
+      <c r="E73" s="14" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="47.25">
-      <c r="B73" s="4" t="s">
+    <row r="74" spans="1:5" ht="45">
+      <c r="B74" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C73" s="2" t="s">
+      <c r="C74" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E73" s="14" t="s">
+      <c r="E74" s="14" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="63">
-      <c r="B74" s="4" t="s">
+    <row r="75" spans="1:5" ht="60">
+      <c r="B75" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="C75" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E74" s="14" t="s">
+      <c r="E75" s="14" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="63">
-      <c r="B75" s="4" t="s">
+    <row r="76" spans="1:5" ht="60">
+      <c r="B76" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="C76" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="E75" s="14" t="s">
+      <c r="E76" s="14" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="105">
-      <c r="A76" s="5"/>
-      <c r="B76" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C76" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D76" s="6"/>
-      <c r="E76" s="5" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" ht="60" customHeight="1">
+    <row r="77" spans="1:5" ht="105">
       <c r="A77" s="5"/>
       <c r="B77" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="C77" s="5"/>
-      <c r="D77" s="5"/>
-      <c r="E77" s="14" t="s">
-        <v>165</v>
+        <v>40</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D77" s="6"/>
+      <c r="E77" s="5" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="60" customHeight="1">
       <c r="A78" s="5"/>
       <c r="B78" s="6" t="s">
-        <v>214</v>
+        <v>100</v>
       </c>
       <c r="C78" s="5"/>
       <c r="D78" s="5"/>
       <c r="E78" s="14" t="s">
-        <v>216</v>
+        <v>165</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="60" customHeight="1">
       <c r="A79" s="5"/>
       <c r="B79" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
       <c r="E79" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="60" customHeight="1">
+      <c r="A80" s="5"/>
+      <c r="B80" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="C80" s="5"/>
+      <c r="D80" s="5"/>
+      <c r="E80" s="14" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="47.25">
-      <c r="A80" s="5" t="s">
+    <row r="81" spans="1:18" ht="45">
+      <c r="A81" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B80" s="4" t="s">
+      <c r="B81" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C80" s="5" t="s">
+      <c r="C81" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D80" s="5"/>
-      <c r="E80" s="5" t="s">
+      <c r="D81" s="5"/>
+      <c r="E81" s="5" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="81" spans="1:18">
-      <c r="A81" s="12" t="s">
+    <row r="82" spans="1:18">
+      <c r="A82" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B81" s="24"/>
-      <c r="C81" s="1"/>
-      <c r="D81" s="1"/>
-      <c r="E81" s="1"/>
-    </row>
-    <row r="82" spans="1:18" s="13" customFormat="1" ht="47.25">
-      <c r="A82" s="6"/>
-      <c r="B82" s="25" t="s">
-        <v>170</v>
-      </c>
-      <c r="C82" s="6"/>
-      <c r="D82" s="22"/>
-      <c r="E82" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="F82" s="23"/>
-      <c r="G82" s="23"/>
-      <c r="H82" s="23"/>
-      <c r="I82" s="4"/>
-      <c r="J82" s="6"/>
-      <c r="K82" s="6"/>
-      <c r="L82" s="6"/>
-      <c r="M82" s="6"/>
-      <c r="N82" s="6"/>
-      <c r="O82" s="6"/>
-      <c r="P82" s="6"/>
-      <c r="Q82" s="6"/>
-      <c r="R82" s="6"/>
-    </row>
-    <row r="83" spans="1:18" s="13" customFormat="1" ht="63">
+      <c r="B82" s="24"/>
+      <c r="C82" s="1"/>
+      <c r="D82" s="1"/>
+      <c r="E82" s="1"/>
+    </row>
+    <row r="83" spans="1:18" s="13" customFormat="1" ht="45">
       <c r="A83" s="6"/>
       <c r="B83" s="25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C83" s="6"/>
       <c r="D83" s="22"/>
       <c r="E83" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F83" s="23"/>
       <c r="G83" s="23"/>
@@ -3906,15 +3901,15 @@
       <c r="Q83" s="6"/>
       <c r="R83" s="6"/>
     </row>
-    <row r="84" spans="1:18" s="13" customFormat="1" ht="47.25">
+    <row r="84" spans="1:18" s="13" customFormat="1" ht="60">
       <c r="A84" s="6"/>
       <c r="B84" s="25" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C84" s="6"/>
       <c r="D84" s="22"/>
       <c r="E84" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F84" s="23"/>
       <c r="G84" s="23"/>
@@ -3930,15 +3925,15 @@
       <c r="Q84" s="6"/>
       <c r="R84" s="6"/>
     </row>
-    <row r="85" spans="1:18" s="13" customFormat="1" ht="47.25">
+    <row r="85" spans="1:18" s="13" customFormat="1" ht="45">
       <c r="A85" s="6"/>
       <c r="B85" s="25" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C85" s="6"/>
       <c r="D85" s="22"/>
       <c r="E85" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F85" s="23"/>
       <c r="G85" s="23"/>
@@ -3954,15 +3949,15 @@
       <c r="Q85" s="6"/>
       <c r="R85" s="6"/>
     </row>
-    <row r="86" spans="1:18" s="13" customFormat="1" ht="63">
+    <row r="86" spans="1:18" s="13" customFormat="1" ht="45">
       <c r="A86" s="6"/>
       <c r="B86" s="25" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C86" s="6"/>
       <c r="D86" s="22"/>
       <c r="E86" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F86" s="23"/>
       <c r="G86" s="23"/>
@@ -3978,15 +3973,15 @@
       <c r="Q86" s="6"/>
       <c r="R86" s="6"/>
     </row>
-    <row r="87" spans="1:18" s="13" customFormat="1" ht="47.25">
+    <row r="87" spans="1:18" s="13" customFormat="1" ht="60">
       <c r="A87" s="6"/>
       <c r="B87" s="25" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C87" s="6"/>
       <c r="D87" s="22"/>
       <c r="E87" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F87" s="23"/>
       <c r="G87" s="23"/>
@@ -4002,118 +3997,142 @@
       <c r="Q87" s="6"/>
       <c r="R87" s="6"/>
     </row>
-    <row r="88" spans="1:18" ht="63">
-      <c r="A88" s="5"/>
-      <c r="B88" s="6" t="s">
-        <v>105</v>
+    <row r="88" spans="1:18" s="13" customFormat="1" ht="45">
+      <c r="A88" s="6"/>
+      <c r="B88" s="25" t="s">
+        <v>175</v>
       </c>
       <c r="C88" s="6"/>
-      <c r="D88" s="11"/>
+      <c r="D88" s="22"/>
       <c r="E88" s="3" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="89" spans="1:18" ht="63">
+        <v>177</v>
+      </c>
+      <c r="F88" s="23"/>
+      <c r="G88" s="23"/>
+      <c r="H88" s="23"/>
+      <c r="I88" s="4"/>
+      <c r="J88" s="6"/>
+      <c r="K88" s="6"/>
+      <c r="L88" s="6"/>
+      <c r="M88" s="6"/>
+      <c r="N88" s="6"/>
+      <c r="O88" s="6"/>
+      <c r="P88" s="6"/>
+      <c r="Q88" s="6"/>
+      <c r="R88" s="6"/>
+    </row>
+    <row r="89" spans="1:18" ht="60">
       <c r="A89" s="5"/>
       <c r="B89" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C89" s="6"/>
       <c r="D89" s="11"/>
       <c r="E89" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="90" spans="1:18" ht="63">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" ht="60">
       <c r="A90" s="5"/>
       <c r="B90" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C90" s="6"/>
+      <c r="D90" s="11"/>
+      <c r="E90" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18" ht="60">
+      <c r="A91" s="5"/>
+      <c r="B91" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C90" s="5" t="s">
+      <c r="C91" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D90" s="5"/>
-      <c r="E90" s="5" t="s">
+      <c r="D91" s="5"/>
+      <c r="E91" s="5" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="91" spans="1:18">
-      <c r="A91" s="12" t="s">
+    <row r="92" spans="1:18">
+      <c r="A92" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="B91" s="24"/>
-      <c r="C91" s="1"/>
-      <c r="D91" s="1"/>
-      <c r="E91" s="1"/>
-    </row>
-    <row r="92" spans="1:18" s="13" customFormat="1" ht="47.25">
-      <c r="B92" s="4" t="s">
+      <c r="B92" s="24"/>
+      <c r="C92" s="1"/>
+      <c r="D92" s="1"/>
+      <c r="E92" s="1"/>
+    </row>
+    <row r="93" spans="1:18" s="13" customFormat="1" ht="45">
+      <c r="B93" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="E92" s="13" t="s">
+      <c r="E93" s="13" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="93" spans="1:18">
-      <c r="A93" s="12" t="s">
+    <row r="94" spans="1:18">
+      <c r="A94" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="B93" s="24"/>
-      <c r="C93" s="1"/>
-      <c r="D93" s="17"/>
-      <c r="E93" s="1"/>
-    </row>
-    <row r="94" spans="1:18" ht="63">
-      <c r="B94" s="13" t="s">
+      <c r="B94" s="24"/>
+      <c r="C94" s="1"/>
+      <c r="D94" s="17"/>
+      <c r="E94" s="1"/>
+    </row>
+    <row r="95" spans="1:18" ht="60">
+      <c r="B95" s="13" t="s">
         <v>137</v>
-      </c>
-      <c r="D94" s="18"/>
-      <c r="E94" s="8" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="95" spans="1:18" ht="63">
-      <c r="B95" s="13" t="s">
-        <v>138</v>
       </c>
       <c r="D95" s="18"/>
       <c r="E95" s="8" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="96" spans="1:18" ht="63">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18" ht="60">
       <c r="B96" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D96" s="18"/>
       <c r="E96" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="97" spans="2:5" ht="63">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="97" spans="2:5" ht="60">
       <c r="B97" s="13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D97" s="18"/>
       <c r="E97" s="8" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="98" spans="2:5" ht="63">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="98" spans="2:5" ht="60">
       <c r="B98" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D98" s="18"/>
       <c r="E98" s="8" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="99" spans="2:5" ht="63">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="99" spans="2:5" ht="60">
       <c r="B99" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D99" s="18"/>
       <c r="E99" s="8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="100" spans="2:5" ht="60">
+      <c r="B100" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="D100" s="18"/>
+      <c r="E100" s="8" t="s">
         <v>145</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated SSP to include booking photo (mugshot) field with the ability to optimize with MTOM
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Custody_Query_Results/artifacts/service_model/information_model/IEPD/documentation/impl/CustodyQueryResults.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Custody_Query_Results/artifacts/service_model/information_model/IEPD/documentation/impl/CustodyQueryResults.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-23860" yWindow="1180" windowWidth="20580" windowHeight="15340" tabRatio="500"/>
+    <workbookView xWindow="5120" yWindow="2560" windowWidth="20580" windowHeight="15340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Custody Query Results Mappin" sheetId="1" r:id="rId1"/>
@@ -324,9 +324,6 @@
     <t>Highest Charge Indicator</t>
   </si>
   <si>
-    <t>/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/nc:Person[@structures:id=/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonDigitalImage/nc:Base64BinaryObject</t>
-  </si>
-  <si>
     <t>Case</t>
   </si>
   <si>
@@ -691,6 +688,9 @@
   </si>
   <si>
     <t>/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/j:Detention[@structures:id=/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/j:ActivityCaseAssociation/nc:Activity/@structures:ref]/j:SupervisionAugmentation/j:SupervisionCondition/nc:ActivityDescriptionText</t>
+  </si>
+  <si>
+    <t>/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/nc:Person[@structures:id=/cq-res-doc:CustodyQueryResults/cq-res-ext:Custody/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonDigitalImage/cq-res-ext:Base64BinaryObject</t>
   </si>
 </sst>
 </file>
@@ -2858,8 +2858,8 @@
   <dimension ref="A1:R100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C66" sqref="C66"/>
+      <pane ySplit="2" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2874,7 +2874,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="20" customFormat="1">
       <c r="A1" s="32" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B1" s="32"/>
       <c r="C1" s="21"/>
@@ -2969,7 +2969,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -2979,12 +2979,12 @@
     <row r="10" spans="1:8" ht="60">
       <c r="A10" s="14"/>
       <c r="B10" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -2999,89 +2999,89 @@
     <row r="12" spans="1:8" s="5" customFormat="1" ht="60">
       <c r="A12" s="15"/>
       <c r="B12" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="5" customFormat="1" ht="45">
       <c r="A13" s="15"/>
       <c r="B13" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="5" customFormat="1" ht="45">
       <c r="A14" s="15"/>
       <c r="B14" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="14" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="5" customFormat="1" ht="45">
       <c r="A15" s="15"/>
       <c r="B15" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="5" customFormat="1" ht="45">
       <c r="A16" s="15"/>
       <c r="B16" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="14" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="5" customFormat="1" ht="60">
       <c r="A17" s="15"/>
       <c r="B17" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="5" customFormat="1" ht="60">
       <c r="A18" s="15"/>
       <c r="B18" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="5" customFormat="1" ht="60">
       <c r="A19" s="15"/>
       <c r="B19" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="60">
@@ -3152,40 +3152,40 @@
     <row r="25" spans="1:5" ht="60">
       <c r="A25" s="10"/>
       <c r="B25" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="60">
       <c r="A26" s="10"/>
       <c r="B26" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="60">
       <c r="A27" s="10"/>
       <c r="B27" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="60">
@@ -3256,25 +3256,25 @@
     <row r="33" spans="1:13" ht="60">
       <c r="A33" s="4"/>
       <c r="B33" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C33" s="4"/>
       <c r="D33" s="10"/>
       <c r="E33" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:13" s="13" customFormat="1" ht="75">
       <c r="A34" s="4"/>
       <c r="B34" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>190</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>191</v>
       </c>
       <c r="D34" s="26"/>
       <c r="E34" s="28" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F34" s="28"/>
       <c r="G34" s="28"/>
@@ -3288,12 +3288,12 @@
     <row r="35" spans="1:13" s="13" customFormat="1" ht="60">
       <c r="A35" s="4"/>
       <c r="B35" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C35" s="4"/>
       <c r="D35" s="26"/>
       <c r="E35" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F35" s="27"/>
       <c r="G35" s="28"/>
@@ -3307,12 +3307,12 @@
     <row r="36" spans="1:13" s="13" customFormat="1" ht="60">
       <c r="A36" s="4"/>
       <c r="B36" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="26"/>
       <c r="E36" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F36" s="27"/>
       <c r="G36" s="28"/>
@@ -3326,12 +3326,12 @@
     <row r="37" spans="1:13" s="13" customFormat="1" ht="60">
       <c r="A37" s="4"/>
       <c r="B37" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="26"/>
       <c r="E37" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F37" s="27"/>
       <c r="G37" s="28"/>
@@ -3345,12 +3345,12 @@
     <row r="38" spans="1:13" s="13" customFormat="1" ht="60">
       <c r="A38" s="4"/>
       <c r="B38" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="26"/>
       <c r="E38" s="8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F38" s="27"/>
       <c r="G38" s="28"/>
@@ -3366,12 +3366,12 @@
         <v>38</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C39" s="4"/>
       <c r="D39" s="26"/>
       <c r="E39" s="8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F39" s="27"/>
       <c r="G39" s="28"/>
@@ -3384,7 +3384,7 @@
     </row>
     <row r="40" spans="1:13" s="13" customFormat="1">
       <c r="A40" s="30" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B40" s="24"/>
       <c r="C40" s="24"/>
@@ -3401,7 +3401,7 @@
       </c>
       <c r="D41" s="8"/>
       <c r="E41" s="31" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="42" spans="1:13" s="13" customFormat="1" ht="60">
@@ -3414,7 +3414,7 @@
       </c>
       <c r="D42" s="8"/>
       <c r="E42" s="31" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="43" spans="1:13" s="13" customFormat="1" ht="60">
@@ -3427,7 +3427,7 @@
       </c>
       <c r="D43" s="8"/>
       <c r="E43" s="31" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="44" spans="1:13" s="13" customFormat="1" ht="60">
@@ -3440,7 +3440,7 @@
       </c>
       <c r="D44" s="8"/>
       <c r="E44" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="45" spans="1:13" s="13" customFormat="1" ht="60">
@@ -3453,7 +3453,7 @@
       </c>
       <c r="D45" s="8"/>
       <c r="E45" s="31" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="46" spans="1:13">
@@ -3512,25 +3512,25 @@
     <row r="51" spans="1:5" s="13" customFormat="1" ht="60">
       <c r="A51" s="29"/>
       <c r="B51" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C51" s="4"/>
       <c r="D51" s="4"/>
       <c r="E51" s="14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="60">
       <c r="A52" s="16"/>
       <c r="B52" s="8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C52" s="14" t="s">
         <v>75</v>
       </c>
       <c r="D52" s="14"/>
       <c r="E52" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="45">
@@ -3543,20 +3543,20 @@
       </c>
       <c r="D53" s="8"/>
       <c r="E53" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="60">
       <c r="A54" s="14"/>
       <c r="B54" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="C54" s="8" t="s">
         <v>184</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>185</v>
       </c>
       <c r="D54" s="8"/>
       <c r="E54" s="14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="60">
@@ -3567,7 +3567,7 @@
         <v>35</v>
       </c>
       <c r="E55" s="14" t="s">
-        <v>101</v>
+        <v>223</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -3614,13 +3614,13 @@
     </row>
     <row r="60" spans="1:5" ht="60">
       <c r="B60" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>45</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="45">
@@ -3631,7 +3631,7 @@
         <v>46</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="60">
@@ -3645,7 +3645,7 @@
         <v>42</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="60">
@@ -3656,40 +3656,40 @@
         <v>82</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="64" spans="1:5" s="13" customFormat="1" ht="60">
       <c r="A64" s="8"/>
       <c r="B64" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C64" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="C64" s="13" t="s">
-        <v>123</v>
-      </c>
       <c r="E64" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="65" spans="1:5" s="13" customFormat="1" ht="60">
       <c r="A65" s="8"/>
       <c r="B65" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="C65" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="C65" s="13" t="s">
-        <v>125</v>
-      </c>
       <c r="E65" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="66" spans="1:5" s="13" customFormat="1" ht="60">
       <c r="A66" s="8"/>
       <c r="B66" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="E66" s="2" t="s">
         <v>222</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="60">
@@ -3702,18 +3702,18 @@
       </c>
       <c r="D67" s="5"/>
       <c r="E67" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="60">
       <c r="A68" s="5"/>
       <c r="B68" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
       <c r="E68" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="60">
@@ -3728,7 +3728,7 @@
       </c>
       <c r="D69" s="5"/>
       <c r="E69" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="45">
@@ -3743,7 +3743,7 @@
       </c>
       <c r="D70" s="5"/>
       <c r="E70" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -3763,15 +3763,15 @@
         <v>78</v>
       </c>
       <c r="E72" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="45">
       <c r="B73" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E73" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="45">
@@ -3782,7 +3782,7 @@
         <v>79</v>
       </c>
       <c r="E74" s="14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="60">
@@ -3793,18 +3793,18 @@
         <v>39</v>
       </c>
       <c r="E75" s="14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="60">
       <c r="B76" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E76" s="14" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="105">
@@ -3817,7 +3817,7 @@
       </c>
       <c r="D77" s="6"/>
       <c r="E77" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="60" customHeight="1">
@@ -3828,29 +3828,29 @@
       <c r="C78" s="5"/>
       <c r="D78" s="5"/>
       <c r="E78" s="14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="60" customHeight="1">
       <c r="A79" s="5"/>
       <c r="B79" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
       <c r="E79" s="14" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="60" customHeight="1">
       <c r="A80" s="5"/>
       <c r="B80" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C80" s="5"/>
       <c r="D80" s="5"/>
       <c r="E80" s="14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="81" spans="1:18" ht="45">
@@ -3865,7 +3865,7 @@
       </c>
       <c r="D81" s="5"/>
       <c r="E81" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="82" spans="1:18">
@@ -3880,12 +3880,12 @@
     <row r="83" spans="1:18" s="13" customFormat="1" ht="45">
       <c r="A83" s="6"/>
       <c r="B83" s="25" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C83" s="6"/>
       <c r="D83" s="22"/>
       <c r="E83" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F83" s="23"/>
       <c r="G83" s="23"/>
@@ -3904,12 +3904,12 @@
     <row r="84" spans="1:18" s="13" customFormat="1" ht="60">
       <c r="A84" s="6"/>
       <c r="B84" s="25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C84" s="6"/>
       <c r="D84" s="22"/>
       <c r="E84" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F84" s="23"/>
       <c r="G84" s="23"/>
@@ -3928,12 +3928,12 @@
     <row r="85" spans="1:18" s="13" customFormat="1" ht="45">
       <c r="A85" s="6"/>
       <c r="B85" s="25" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C85" s="6"/>
       <c r="D85" s="22"/>
       <c r="E85" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F85" s="23"/>
       <c r="G85" s="23"/>
@@ -3952,12 +3952,12 @@
     <row r="86" spans="1:18" s="13" customFormat="1" ht="45">
       <c r="A86" s="6"/>
       <c r="B86" s="25" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C86" s="6"/>
       <c r="D86" s="22"/>
       <c r="E86" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F86" s="23"/>
       <c r="G86" s="23"/>
@@ -3976,12 +3976,12 @@
     <row r="87" spans="1:18" s="13" customFormat="1" ht="60">
       <c r="A87" s="6"/>
       <c r="B87" s="25" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C87" s="6"/>
       <c r="D87" s="22"/>
       <c r="E87" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F87" s="23"/>
       <c r="G87" s="23"/>
@@ -4000,12 +4000,12 @@
     <row r="88" spans="1:18" s="13" customFormat="1" ht="45">
       <c r="A88" s="6"/>
       <c r="B88" s="25" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C88" s="6"/>
       <c r="D88" s="22"/>
       <c r="E88" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F88" s="23"/>
       <c r="G88" s="23"/>
@@ -4024,23 +4024,23 @@
     <row r="89" spans="1:18" ht="60">
       <c r="A89" s="5"/>
       <c r="B89" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C89" s="6"/>
       <c r="D89" s="11"/>
       <c r="E89" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="90" spans="1:18" ht="60">
       <c r="A90" s="5"/>
       <c r="B90" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C90" s="6"/>
       <c r="D90" s="11"/>
       <c r="E90" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="91" spans="1:18" ht="60">
@@ -4053,12 +4053,12 @@
       </c>
       <c r="D91" s="5"/>
       <c r="E91" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="92" spans="1:18">
       <c r="A92" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B92" s="24"/>
       <c r="C92" s="1"/>
@@ -4067,15 +4067,15 @@
     </row>
     <row r="93" spans="1:18" s="13" customFormat="1" ht="45">
       <c r="B93" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E93" s="13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="94" spans="1:18">
       <c r="A94" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B94" s="24"/>
       <c r="C94" s="1"/>
@@ -4084,56 +4084,56 @@
     </row>
     <row r="95" spans="1:18" ht="60">
       <c r="B95" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D95" s="18"/>
       <c r="E95" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="96" spans="1:18" ht="60">
       <c r="B96" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D96" s="18"/>
       <c r="E96" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="97" spans="2:5" ht="60">
       <c r="B97" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D97" s="18"/>
       <c r="E97" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="98" spans="2:5" ht="60">
       <c r="B98" s="13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D98" s="18"/>
       <c r="E98" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="99" spans="2:5" ht="60">
       <c r="B99" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D99" s="18"/>
       <c r="E99" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="100" spans="2:5" ht="60">
       <c r="B100" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D100" s="18"/>
       <c r="E100" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>